<commit_message>
remove Patient cardinality 0..0 from bundle dccb9dc5fb5dc4579e1743d23a73fbf6951c3dc5
</commit_message>
<xml_diff>
--- a/ig/nr-change-contained/StructureDefinition-pdsm-comprehensive-document-reference.xlsx
+++ b/ig/nr-change-contained/StructureDefinition-pdsm-comprehensive-document-reference.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3100" uniqueCount="581">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3099" uniqueCount="580">
   <si>
     <t>Property</t>
   </si>
@@ -60,7 +60,7 @@
     <t>Date</t>
   </si>
   <si>
-    <t>2023-07-12T08:12:47+00:00</t>
+    <t>2023-07-12T08:15:17+00:00</t>
   </si>
   <si>
     <t>Publisher</t>
@@ -685,9 +685,6 @@
   </si>
   <si>
     <t>Key metadata element describing the document that describes he exact type of document. Helps humans to assess whether the document is of interest when viewing a list of documents.</t>
-  </si>
-  <si>
-    <t>XDS typeCode CI-SIS</t>
   </si>
   <si>
     <t>https://mos.esante.gouv.fr/NOS/JDV_J07-XdsTypeCode-CISIS/FHIR/JDV-J07-XdsTypeCode-CISIS</t>
@@ -5246,11 +5243,9 @@
       <c r="X24" t="s" s="2">
         <v>131</v>
       </c>
-      <c r="Y24" t="s" s="2">
+      <c r="Y24" s="2"/>
+      <c r="Z24" t="s" s="2">
         <v>214</v>
-      </c>
-      <c r="Z24" t="s" s="2">
-        <v>215</v>
       </c>
       <c r="AA24" t="s" s="2">
         <v>35</v>
@@ -5280,46 +5275,46 @@
         <v>35</v>
       </c>
       <c r="AJ24" t="s" s="2">
+        <v>215</v>
+      </c>
+      <c r="AK24" t="s" s="2">
         <v>216</v>
       </c>
-      <c r="AK24" t="s" s="2">
+      <c r="AL24" t="s" s="2">
         <v>217</v>
       </c>
-      <c r="AL24" t="s" s="2">
+      <c r="AM24" t="s" s="2">
         <v>218</v>
       </c>
-      <c r="AM24" t="s" s="2">
+      <c r="AN24" t="s" s="2">
         <v>219</v>
       </c>
-      <c r="AN24" t="s" s="2">
+      <c r="AO24" t="s" s="2">
         <v>220</v>
       </c>
-      <c r="AO24" t="s" s="2">
+      <c r="AP24" t="s" s="2">
         <v>221</v>
       </c>
-      <c r="AP24" t="s" s="2">
+      <c r="AQ24" t="s" s="2">
         <v>222</v>
       </c>
-      <c r="AQ24" t="s" s="2">
+      <c r="AR24" t="s" s="2">
         <v>223</v>
       </c>
-      <c r="AR24" t="s" s="2">
+      <c r="AS24" t="s" s="2">
         <v>224</v>
-      </c>
-      <c r="AS24" t="s" s="2">
-        <v>225</v>
       </c>
     </row>
     <row r="25" hidden="true">
       <c r="A25" t="s" s="2">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="B25" t="s" s="2">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="C25" s="2"/>
       <c r="D25" t="s" s="2">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="E25" s="2"/>
       <c r="F25" t="s" s="2">
@@ -5341,13 +5336,13 @@
         <v>210</v>
       </c>
       <c r="L25" t="s" s="2">
+        <v>227</v>
+      </c>
+      <c r="M25" t="s" s="2">
         <v>228</v>
       </c>
-      <c r="M25" t="s" s="2">
+      <c r="N25" t="s" s="2">
         <v>229</v>
-      </c>
-      <c r="N25" t="s" s="2">
-        <v>230</v>
       </c>
       <c r="O25" s="2"/>
       <c r="P25" t="s" s="2">
@@ -5376,11 +5371,11 @@
         <v>131</v>
       </c>
       <c r="Y25" t="s" s="2">
+        <v>230</v>
+      </c>
+      <c r="Z25" t="s" s="2">
         <v>231</v>
       </c>
-      <c r="Z25" t="s" s="2">
-        <v>232</v>
-      </c>
       <c r="AA25" t="s" s="2">
         <v>35</v>
       </c>
@@ -5397,7 +5392,7 @@
         <v>35</v>
       </c>
       <c r="AF25" t="s" s="2">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="AG25" t="s" s="2">
         <v>36</v>
@@ -5409,42 +5404,42 @@
         <v>35</v>
       </c>
       <c r="AJ25" t="s" s="2">
+        <v>232</v>
+      </c>
+      <c r="AK25" t="s" s="2">
+        <v>35</v>
+      </c>
+      <c r="AL25" t="s" s="2">
         <v>233</v>
       </c>
-      <c r="AK25" t="s" s="2">
-        <v>35</v>
-      </c>
-      <c r="AL25" t="s" s="2">
+      <c r="AM25" t="s" s="2">
         <v>234</v>
       </c>
-      <c r="AM25" t="s" s="2">
+      <c r="AN25" t="s" s="2">
         <v>235</v>
       </c>
-      <c r="AN25" t="s" s="2">
+      <c r="AO25" t="s" s="2">
+        <v>220</v>
+      </c>
+      <c r="AP25" t="s" s="2">
+        <v>35</v>
+      </c>
+      <c r="AQ25" t="s" s="2">
         <v>236</v>
       </c>
-      <c r="AO25" t="s" s="2">
-        <v>221</v>
-      </c>
-      <c r="AP25" t="s" s="2">
-        <v>35</v>
-      </c>
-      <c r="AQ25" t="s" s="2">
+      <c r="AR25" t="s" s="2">
         <v>237</v>
       </c>
-      <c r="AR25" t="s" s="2">
+      <c r="AS25" t="s" s="2">
         <v>238</v>
-      </c>
-      <c r="AS25" t="s" s="2">
-        <v>239</v>
       </c>
     </row>
     <row r="26" hidden="true">
       <c r="A26" t="s" s="2">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="B26" t="s" s="2">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="C26" s="2"/>
       <c r="D26" t="s" s="2">
@@ -5467,13 +5462,13 @@
         <v>50</v>
       </c>
       <c r="K26" t="s" s="2">
+        <v>240</v>
+      </c>
+      <c r="L26" t="s" s="2">
         <v>241</v>
       </c>
-      <c r="L26" t="s" s="2">
+      <c r="M26" t="s" s="2">
         <v>242</v>
-      </c>
-      <c r="M26" t="s" s="2">
-        <v>243</v>
       </c>
       <c r="N26" s="2"/>
       <c r="O26" s="2"/>
@@ -5524,7 +5519,7 @@
         <v>35</v>
       </c>
       <c r="AF26" t="s" s="2">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="AG26" t="s" s="2">
         <v>36</v>
@@ -5536,46 +5531,46 @@
         <v>35</v>
       </c>
       <c r="AJ26" t="s" s="2">
+        <v>243</v>
+      </c>
+      <c r="AK26" t="s" s="2">
         <v>244</v>
       </c>
-      <c r="AK26" t="s" s="2">
+      <c r="AL26" t="s" s="2">
         <v>245</v>
       </c>
-      <c r="AL26" t="s" s="2">
+      <c r="AM26" t="s" s="2">
         <v>246</v>
       </c>
-      <c r="AM26" t="s" s="2">
+      <c r="AN26" t="s" s="2">
         <v>247</v>
       </c>
-      <c r="AN26" t="s" s="2">
+      <c r="AO26" t="s" s="2">
         <v>248</v>
       </c>
-      <c r="AO26" t="s" s="2">
+      <c r="AP26" t="s" s="2">
         <v>249</v>
       </c>
-      <c r="AP26" t="s" s="2">
+      <c r="AQ26" t="s" s="2">
         <v>250</v>
       </c>
-      <c r="AQ26" t="s" s="2">
+      <c r="AR26" t="s" s="2">
+        <v>250</v>
+      </c>
+      <c r="AS26" t="s" s="2">
         <v>251</v>
-      </c>
-      <c r="AR26" t="s" s="2">
-        <v>251</v>
-      </c>
-      <c r="AS26" t="s" s="2">
-        <v>252</v>
       </c>
     </row>
     <row r="27" hidden="true">
       <c r="A27" t="s" s="2">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="B27" t="s" s="2">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="C27" s="2"/>
       <c r="D27" t="s" s="2">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="E27" s="2"/>
       <c r="F27" t="s" s="2">
@@ -5597,13 +5592,13 @@
         <v>86</v>
       </c>
       <c r="L27" t="s" s="2">
+        <v>254</v>
+      </c>
+      <c r="M27" t="s" s="2">
         <v>255</v>
       </c>
-      <c r="M27" t="s" s="2">
+      <c r="N27" t="s" s="2">
         <v>256</v>
-      </c>
-      <c r="N27" t="s" s="2">
-        <v>257</v>
       </c>
       <c r="O27" s="2"/>
       <c r="P27" t="s" s="2">
@@ -5653,7 +5648,7 @@
         <v>35</v>
       </c>
       <c r="AF27" t="s" s="2">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="AG27" t="s" s="2">
         <v>36</v>
@@ -5668,19 +5663,19 @@
         <v>83</v>
       </c>
       <c r="AK27" t="s" s="2">
+        <v>257</v>
+      </c>
+      <c r="AL27" t="s" s="2">
         <v>258</v>
       </c>
-      <c r="AL27" t="s" s="2">
+      <c r="AM27" t="s" s="2">
         <v>259</v>
       </c>
-      <c r="AM27" t="s" s="2">
+      <c r="AN27" t="s" s="2">
+        <v>35</v>
+      </c>
+      <c r="AO27" t="s" s="2">
         <v>260</v>
-      </c>
-      <c r="AN27" t="s" s="2">
-        <v>35</v>
-      </c>
-      <c r="AO27" t="s" s="2">
-        <v>261</v>
       </c>
       <c r="AP27" t="s" s="2">
         <v>35</v>
@@ -5697,10 +5692,10 @@
     </row>
     <row r="28" hidden="true">
       <c r="A28" t="s" s="2">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="B28" t="s" s="2">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="C28" s="2"/>
       <c r="D28" t="s" s="2">
@@ -5723,16 +5718,16 @@
         <v>50</v>
       </c>
       <c r="K28" t="s" s="2">
+        <v>262</v>
+      </c>
+      <c r="L28" t="s" s="2">
         <v>263</v>
       </c>
-      <c r="L28" t="s" s="2">
+      <c r="M28" t="s" s="2">
         <v>264</v>
       </c>
-      <c r="M28" t="s" s="2">
+      <c r="N28" t="s" s="2">
         <v>265</v>
-      </c>
-      <c r="N28" t="s" s="2">
-        <v>266</v>
       </c>
       <c r="O28" s="2"/>
       <c r="P28" t="s" s="2">
@@ -5782,7 +5777,7 @@
         <v>35</v>
       </c>
       <c r="AF28" t="s" s="2">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="AG28" t="s" s="2">
         <v>36</v>
@@ -5794,42 +5789,42 @@
         <v>35</v>
       </c>
       <c r="AJ28" t="s" s="2">
+        <v>266</v>
+      </c>
+      <c r="AK28" t="s" s="2">
         <v>267</v>
       </c>
-      <c r="AK28" t="s" s="2">
+      <c r="AL28" t="s" s="2">
         <v>268</v>
       </c>
-      <c r="AL28" t="s" s="2">
+      <c r="AM28" t="s" s="2">
         <v>269</v>
       </c>
-      <c r="AM28" t="s" s="2">
+      <c r="AN28" t="s" s="2">
         <v>270</v>
       </c>
-      <c r="AN28" t="s" s="2">
+      <c r="AO28" t="s" s="2">
+        <v>35</v>
+      </c>
+      <c r="AP28" t="s" s="2">
         <v>271</v>
       </c>
-      <c r="AO28" t="s" s="2">
-        <v>35</v>
-      </c>
-      <c r="AP28" t="s" s="2">
+      <c r="AQ28" t="s" s="2">
         <v>272</v>
       </c>
-      <c r="AQ28" t="s" s="2">
+      <c r="AR28" t="s" s="2">
+        <v>272</v>
+      </c>
+      <c r="AS28" t="s" s="2">
         <v>273</v>
-      </c>
-      <c r="AR28" t="s" s="2">
-        <v>273</v>
-      </c>
-      <c r="AS28" t="s" s="2">
-        <v>274</v>
       </c>
     </row>
     <row r="29" hidden="true">
       <c r="A29" t="s" s="2">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="B29" t="s" s="2">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="C29" s="2"/>
       <c r="D29" t="s" s="2">
@@ -5852,16 +5847,16 @@
         <v>35</v>
       </c>
       <c r="K29" t="s" s="2">
+        <v>275</v>
+      </c>
+      <c r="L29" t="s" s="2">
         <v>276</v>
       </c>
-      <c r="L29" t="s" s="2">
+      <c r="M29" t="s" s="2">
         <v>277</v>
       </c>
-      <c r="M29" t="s" s="2">
+      <c r="N29" t="s" s="2">
         <v>278</v>
-      </c>
-      <c r="N29" t="s" s="2">
-        <v>279</v>
       </c>
       <c r="O29" s="2"/>
       <c r="P29" t="s" s="2">
@@ -5911,7 +5906,7 @@
         <v>35</v>
       </c>
       <c r="AF29" t="s" s="2">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="AG29" t="s" s="2">
         <v>36</v>
@@ -5923,42 +5918,42 @@
         <v>35</v>
       </c>
       <c r="AJ29" t="s" s="2">
+        <v>279</v>
+      </c>
+      <c r="AK29" t="s" s="2">
+        <v>267</v>
+      </c>
+      <c r="AL29" t="s" s="2">
         <v>280</v>
       </c>
-      <c r="AK29" t="s" s="2">
-        <v>268</v>
-      </c>
-      <c r="AL29" t="s" s="2">
+      <c r="AM29" t="s" s="2">
         <v>281</v>
       </c>
-      <c r="AM29" t="s" s="2">
+      <c r="AN29" t="s" s="2">
         <v>282</v>
       </c>
-      <c r="AN29" t="s" s="2">
+      <c r="AO29" t="s" s="2">
         <v>283</v>
       </c>
-      <c r="AO29" t="s" s="2">
+      <c r="AP29" t="s" s="2">
         <v>284</v>
       </c>
-      <c r="AP29" t="s" s="2">
+      <c r="AQ29" t="s" s="2">
         <v>285</v>
       </c>
-      <c r="AQ29" t="s" s="2">
+      <c r="AR29" t="s" s="2">
+        <v>285</v>
+      </c>
+      <c r="AS29" t="s" s="2">
         <v>286</v>
-      </c>
-      <c r="AR29" t="s" s="2">
-        <v>286</v>
-      </c>
-      <c r="AS29" t="s" s="2">
-        <v>287</v>
       </c>
     </row>
     <row r="30" hidden="true">
       <c r="A30" t="s" s="2">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="B30" t="s" s="2">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="C30" s="2"/>
       <c r="D30" t="s" s="2">
@@ -5981,16 +5976,16 @@
         <v>35</v>
       </c>
       <c r="K30" t="s" s="2">
+        <v>288</v>
+      </c>
+      <c r="L30" t="s" s="2">
         <v>289</v>
       </c>
-      <c r="L30" t="s" s="2">
+      <c r="M30" t="s" s="2">
         <v>290</v>
       </c>
-      <c r="M30" t="s" s="2">
+      <c r="N30" t="s" s="2">
         <v>291</v>
-      </c>
-      <c r="N30" t="s" s="2">
-        <v>292</v>
       </c>
       <c r="O30" s="2"/>
       <c r="P30" t="s" s="2">
@@ -6040,7 +6035,7 @@
         <v>35</v>
       </c>
       <c r="AF30" t="s" s="2">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="AG30" t="s" s="2">
         <v>36</v>
@@ -6055,28 +6050,28 @@
         <v>83</v>
       </c>
       <c r="AK30" t="s" s="2">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="AL30" t="s" s="2">
+        <v>292</v>
+      </c>
+      <c r="AM30" t="s" s="2">
         <v>293</v>
       </c>
-      <c r="AM30" t="s" s="2">
+      <c r="AN30" t="s" s="2">
+        <v>35</v>
+      </c>
+      <c r="AO30" t="s" s="2">
+        <v>35</v>
+      </c>
+      <c r="AP30" t="s" s="2">
+        <v>35</v>
+      </c>
+      <c r="AQ30" t="s" s="2">
+        <v>35</v>
+      </c>
+      <c r="AR30" t="s" s="2">
         <v>294</v>
-      </c>
-      <c r="AN30" t="s" s="2">
-        <v>35</v>
-      </c>
-      <c r="AO30" t="s" s="2">
-        <v>35</v>
-      </c>
-      <c r="AP30" t="s" s="2">
-        <v>35</v>
-      </c>
-      <c r="AQ30" t="s" s="2">
-        <v>35</v>
-      </c>
-      <c r="AR30" t="s" s="2">
-        <v>295</v>
       </c>
       <c r="AS30" t="s" s="2">
         <v>35</v>
@@ -6084,10 +6079,10 @@
     </row>
     <row r="31" hidden="true">
       <c r="A31" t="s" s="2">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="B31" t="s" s="2">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="C31" s="2"/>
       <c r="D31" t="s" s="2">
@@ -6110,16 +6105,16 @@
         <v>50</v>
       </c>
       <c r="K31" t="s" s="2">
+        <v>296</v>
+      </c>
+      <c r="L31" t="s" s="2">
         <v>297</v>
       </c>
-      <c r="L31" t="s" s="2">
+      <c r="M31" t="s" s="2">
         <v>298</v>
       </c>
-      <c r="M31" t="s" s="2">
+      <c r="N31" t="s" s="2">
         <v>299</v>
-      </c>
-      <c r="N31" t="s" s="2">
-        <v>300</v>
       </c>
       <c r="O31" s="2"/>
       <c r="P31" t="s" s="2">
@@ -6169,7 +6164,7 @@
         <v>35</v>
       </c>
       <c r="AF31" t="s" s="2">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="AG31" t="s" s="2">
         <v>36</v>
@@ -6181,31 +6176,31 @@
         <v>35</v>
       </c>
       <c r="AJ31" t="s" s="2">
+        <v>300</v>
+      </c>
+      <c r="AK31" t="s" s="2">
+        <v>35</v>
+      </c>
+      <c r="AL31" t="s" s="2">
         <v>301</v>
       </c>
-      <c r="AK31" t="s" s="2">
-        <v>35</v>
-      </c>
-      <c r="AL31" t="s" s="2">
+      <c r="AM31" t="s" s="2">
         <v>302</v>
       </c>
-      <c r="AM31" t="s" s="2">
+      <c r="AN31" t="s" s="2">
+        <v>35</v>
+      </c>
+      <c r="AO31" t="s" s="2">
+        <v>35</v>
+      </c>
+      <c r="AP31" t="s" s="2">
+        <v>35</v>
+      </c>
+      <c r="AQ31" t="s" s="2">
         <v>303</v>
       </c>
-      <c r="AN31" t="s" s="2">
-        <v>35</v>
-      </c>
-      <c r="AO31" t="s" s="2">
-        <v>35</v>
-      </c>
-      <c r="AP31" t="s" s="2">
-        <v>35</v>
-      </c>
-      <c r="AQ31" t="s" s="2">
-        <v>304</v>
-      </c>
       <c r="AR31" t="s" s="2">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="AS31" t="s" s="2">
         <v>35</v>
@@ -6213,10 +6208,10 @@
     </row>
     <row r="32" hidden="true">
       <c r="A32" t="s" s="2">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="B32" t="s" s="2">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="C32" s="2"/>
       <c r="D32" t="s" s="2">
@@ -6340,10 +6335,10 @@
     </row>
     <row r="33" hidden="true">
       <c r="A33" t="s" s="2">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="B33" t="s" s="2">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="C33" s="2"/>
       <c r="D33" t="s" s="2">
@@ -6469,14 +6464,14 @@
     </row>
     <row r="34" hidden="true">
       <c r="A34" t="s" s="2">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="B34" t="s" s="2">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="C34" s="2"/>
       <c r="D34" t="s" s="2">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="E34" s="2"/>
       <c r="F34" t="s" s="2">
@@ -6498,16 +6493,16 @@
         <v>69</v>
       </c>
       <c r="L34" t="s" s="2">
+        <v>308</v>
+      </c>
+      <c r="M34" t="s" s="2">
         <v>309</v>
-      </c>
-      <c r="M34" t="s" s="2">
-        <v>310</v>
       </c>
       <c r="N34" t="s" s="2">
         <v>72</v>
       </c>
       <c r="O34" t="s" s="2">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="P34" t="s" s="2">
         <v>35</v>
@@ -6556,7 +6551,7 @@
         <v>35</v>
       </c>
       <c r="AF34" t="s" s="2">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="AG34" t="s" s="2">
         <v>36</v>
@@ -6600,10 +6595,10 @@
     </row>
     <row r="35" hidden="true">
       <c r="A35" t="s" s="2">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="B35" t="s" s="2">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="C35" s="2"/>
       <c r="D35" t="s" s="2">
@@ -6629,13 +6624,13 @@
         <v>127</v>
       </c>
       <c r="L35" t="s" s="2">
+        <v>313</v>
+      </c>
+      <c r="M35" t="s" s="2">
         <v>314</v>
       </c>
-      <c r="M35" t="s" s="2">
+      <c r="N35" t="s" s="2">
         <v>315</v>
-      </c>
-      <c r="N35" t="s" s="2">
-        <v>316</v>
       </c>
       <c r="O35" s="2"/>
       <c r="P35" t="s" s="2">
@@ -6664,11 +6659,11 @@
         <v>193</v>
       </c>
       <c r="Y35" t="s" s="2">
+        <v>316</v>
+      </c>
+      <c r="Z35" t="s" s="2">
         <v>317</v>
       </c>
-      <c r="Z35" t="s" s="2">
-        <v>318</v>
-      </c>
       <c r="AA35" t="s" s="2">
         <v>35</v>
       </c>
@@ -6685,7 +6680,7 @@
         <v>35</v>
       </c>
       <c r="AF35" t="s" s="2">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="AG35" t="s" s="2">
         <v>49</v>
@@ -6703,36 +6698,36 @@
         <v>35</v>
       </c>
       <c r="AL35" t="s" s="2">
+        <v>318</v>
+      </c>
+      <c r="AM35" t="s" s="2">
         <v>319</v>
       </c>
-      <c r="AM35" t="s" s="2">
+      <c r="AN35" t="s" s="2">
+        <v>35</v>
+      </c>
+      <c r="AO35" t="s" s="2">
+        <v>35</v>
+      </c>
+      <c r="AP35" t="s" s="2">
+        <v>35</v>
+      </c>
+      <c r="AQ35" t="s" s="2">
         <v>320</v>
       </c>
-      <c r="AN35" t="s" s="2">
-        <v>35</v>
-      </c>
-      <c r="AO35" t="s" s="2">
-        <v>35</v>
-      </c>
-      <c r="AP35" t="s" s="2">
-        <v>35</v>
-      </c>
-      <c r="AQ35" t="s" s="2">
+      <c r="AR35" t="s" s="2">
         <v>321</v>
       </c>
-      <c r="AR35" t="s" s="2">
+      <c r="AS35" t="s" s="2">
         <v>322</v>
-      </c>
-      <c r="AS35" t="s" s="2">
-        <v>323</v>
       </c>
     </row>
     <row r="36" hidden="true">
       <c r="A36" t="s" s="2">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="B36" t="s" s="2">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="C36" s="2"/>
       <c r="D36" t="s" s="2">
@@ -6755,13 +6750,13 @@
         <v>50</v>
       </c>
       <c r="K36" t="s" s="2">
+        <v>324</v>
+      </c>
+      <c r="L36" t="s" s="2">
         <v>325</v>
       </c>
-      <c r="L36" t="s" s="2">
+      <c r="M36" t="s" s="2">
         <v>326</v>
-      </c>
-      <c r="M36" t="s" s="2">
-        <v>327</v>
       </c>
       <c r="N36" s="2"/>
       <c r="O36" s="2"/>
@@ -6812,7 +6807,7 @@
         <v>35</v>
       </c>
       <c r="AF36" t="s" s="2">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="AG36" t="s" s="2">
         <v>49</v>
@@ -6824,42 +6819,42 @@
         <v>35</v>
       </c>
       <c r="AJ36" t="s" s="2">
+        <v>327</v>
+      </c>
+      <c r="AK36" t="s" s="2">
+        <v>35</v>
+      </c>
+      <c r="AL36" t="s" s="2">
         <v>328</v>
       </c>
-      <c r="AK36" t="s" s="2">
-        <v>35</v>
-      </c>
-      <c r="AL36" t="s" s="2">
+      <c r="AM36" t="s" s="2">
         <v>329</v>
       </c>
-      <c r="AM36" t="s" s="2">
+      <c r="AN36" t="s" s="2">
+        <v>35</v>
+      </c>
+      <c r="AO36" t="s" s="2">
+        <v>35</v>
+      </c>
+      <c r="AP36" t="s" s="2">
+        <v>35</v>
+      </c>
+      <c r="AQ36" t="s" s="2">
         <v>330</v>
       </c>
-      <c r="AN36" t="s" s="2">
-        <v>35</v>
-      </c>
-      <c r="AO36" t="s" s="2">
-        <v>35</v>
-      </c>
-      <c r="AP36" t="s" s="2">
-        <v>35</v>
-      </c>
-      <c r="AQ36" t="s" s="2">
+      <c r="AR36" t="s" s="2">
         <v>331</v>
       </c>
-      <c r="AR36" t="s" s="2">
+      <c r="AS36" t="s" s="2">
         <v>332</v>
-      </c>
-      <c r="AS36" t="s" s="2">
-        <v>333</v>
       </c>
     </row>
     <row r="37" hidden="true">
       <c r="A37" t="s" s="2">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="B37" t="s" s="2">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="C37" s="2"/>
       <c r="D37" t="s" s="2">
@@ -6885,16 +6880,16 @@
         <v>62</v>
       </c>
       <c r="L37" t="s" s="2">
+        <v>334</v>
+      </c>
+      <c r="M37" t="s" s="2">
         <v>335</v>
       </c>
-      <c r="M37" t="s" s="2">
+      <c r="N37" t="s" s="2">
         <v>336</v>
       </c>
-      <c r="N37" t="s" s="2">
+      <c r="O37" t="s" s="2">
         <v>337</v>
-      </c>
-      <c r="O37" t="s" s="2">
-        <v>338</v>
       </c>
       <c r="P37" t="s" s="2">
         <v>35</v>
@@ -6943,7 +6938,7 @@
         <v>35</v>
       </c>
       <c r="AF37" t="s" s="2">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="AG37" t="s" s="2">
         <v>36</v>
@@ -6964,33 +6959,33 @@
         <v>35</v>
       </c>
       <c r="AM37" t="s" s="2">
+        <v>338</v>
+      </c>
+      <c r="AN37" t="s" s="2">
+        <v>35</v>
+      </c>
+      <c r="AO37" t="s" s="2">
+        <v>35</v>
+      </c>
+      <c r="AP37" t="s" s="2">
         <v>339</v>
       </c>
-      <c r="AN37" t="s" s="2">
-        <v>35</v>
-      </c>
-      <c r="AO37" t="s" s="2">
-        <v>35</v>
-      </c>
-      <c r="AP37" t="s" s="2">
+      <c r="AQ37" t="s" s="2">
         <v>340</v>
       </c>
-      <c r="AQ37" t="s" s="2">
+      <c r="AR37" t="s" s="2">
+        <v>340</v>
+      </c>
+      <c r="AS37" t="s" s="2">
         <v>341</v>
-      </c>
-      <c r="AR37" t="s" s="2">
-        <v>341</v>
-      </c>
-      <c r="AS37" t="s" s="2">
-        <v>342</v>
       </c>
     </row>
     <row r="38" hidden="true">
       <c r="A38" t="s" s="2">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="B38" t="s" s="2">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="C38" s="2"/>
       <c r="D38" t="s" s="2">
@@ -7016,16 +7011,16 @@
         <v>210</v>
       </c>
       <c r="L38" t="s" s="2">
+        <v>343</v>
+      </c>
+      <c r="M38" t="s" s="2">
         <v>344</v>
       </c>
-      <c r="M38" t="s" s="2">
+      <c r="N38" t="s" s="2">
         <v>345</v>
       </c>
-      <c r="N38" t="s" s="2">
+      <c r="O38" t="s" s="2">
         <v>346</v>
-      </c>
-      <c r="O38" t="s" s="2">
-        <v>347</v>
       </c>
       <c r="P38" t="s" s="2">
         <v>35</v>
@@ -7074,7 +7069,7 @@
         <v>35</v>
       </c>
       <c r="AF38" t="s" s="2">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="AG38" t="s" s="2">
         <v>36</v>
@@ -7086,42 +7081,42 @@
         <v>35</v>
       </c>
       <c r="AJ38" t="s" s="2">
+        <v>347</v>
+      </c>
+      <c r="AK38" t="s" s="2">
+        <v>35</v>
+      </c>
+      <c r="AL38" t="s" s="2">
         <v>348</v>
       </c>
-      <c r="AK38" t="s" s="2">
-        <v>35</v>
-      </c>
-      <c r="AL38" t="s" s="2">
+      <c r="AM38" t="s" s="2">
         <v>349</v>
       </c>
-      <c r="AM38" t="s" s="2">
+      <c r="AN38" t="s" s="2">
         <v>350</v>
       </c>
-      <c r="AN38" t="s" s="2">
+      <c r="AO38" t="s" s="2">
+        <v>35</v>
+      </c>
+      <c r="AP38" t="s" s="2">
         <v>351</v>
       </c>
-      <c r="AO38" t="s" s="2">
-        <v>35</v>
-      </c>
-      <c r="AP38" t="s" s="2">
+      <c r="AQ38" t="s" s="2">
         <v>352</v>
       </c>
-      <c r="AQ38" t="s" s="2">
+      <c r="AR38" t="s" s="2">
+        <v>352</v>
+      </c>
+      <c r="AS38" t="s" s="2">
         <v>353</v>
-      </c>
-      <c r="AR38" t="s" s="2">
-        <v>353</v>
-      </c>
-      <c r="AS38" t="s" s="2">
-        <v>354</v>
       </c>
     </row>
     <row r="39" hidden="true">
       <c r="A39" t="s" s="2">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="B39" t="s" s="2">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="C39" s="2"/>
       <c r="D39" t="s" s="2">
@@ -7144,13 +7139,13 @@
         <v>50</v>
       </c>
       <c r="K39" t="s" s="2">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="L39" t="s" s="2">
+        <v>355</v>
+      </c>
+      <c r="M39" t="s" s="2">
         <v>356</v>
-      </c>
-      <c r="M39" t="s" s="2">
-        <v>357</v>
       </c>
       <c r="N39" s="2"/>
       <c r="O39" s="2"/>
@@ -7201,7 +7196,7 @@
         <v>35</v>
       </c>
       <c r="AF39" t="s" s="2">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="AG39" t="s" s="2">
         <v>49</v>
@@ -7219,10 +7214,10 @@
         <v>35</v>
       </c>
       <c r="AL39" t="s" s="2">
+        <v>357</v>
+      </c>
+      <c r="AM39" t="s" s="2">
         <v>358</v>
-      </c>
-      <c r="AM39" t="s" s="2">
-        <v>359</v>
       </c>
       <c r="AN39" t="s" s="2">
         <v>35</v>
@@ -7245,10 +7240,10 @@
     </row>
     <row r="40" hidden="true">
       <c r="A40" t="s" s="2">
-        <v>360</v>
+        <v>359</v>
       </c>
       <c r="B40" t="s" s="2">
-        <v>360</v>
+        <v>359</v>
       </c>
       <c r="C40" s="2"/>
       <c r="D40" t="s" s="2">
@@ -7372,10 +7367,10 @@
     </row>
     <row r="41" hidden="true">
       <c r="A41" t="s" s="2">
-        <v>361</v>
+        <v>360</v>
       </c>
       <c r="B41" t="s" s="2">
-        <v>361</v>
+        <v>360</v>
       </c>
       <c r="C41" s="2"/>
       <c r="D41" t="s" s="2">
@@ -7501,14 +7496,14 @@
     </row>
     <row r="42" hidden="true">
       <c r="A42" t="s" s="2">
-        <v>362</v>
+        <v>361</v>
       </c>
       <c r="B42" t="s" s="2">
-        <v>362</v>
+        <v>361</v>
       </c>
       <c r="C42" s="2"/>
       <c r="D42" t="s" s="2">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="E42" s="2"/>
       <c r="F42" t="s" s="2">
@@ -7530,16 +7525,16 @@
         <v>69</v>
       </c>
       <c r="L42" t="s" s="2">
+        <v>308</v>
+      </c>
+      <c r="M42" t="s" s="2">
         <v>309</v>
-      </c>
-      <c r="M42" t="s" s="2">
-        <v>310</v>
       </c>
       <c r="N42" t="s" s="2">
         <v>72</v>
       </c>
       <c r="O42" t="s" s="2">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="P42" t="s" s="2">
         <v>35</v>
@@ -7588,7 +7583,7 @@
         <v>35</v>
       </c>
       <c r="AF42" t="s" s="2">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="AG42" t="s" s="2">
         <v>36</v>
@@ -7632,10 +7627,10 @@
     </row>
     <row r="43" hidden="true">
       <c r="A43" t="s" s="2">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="B43" t="s" s="2">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="C43" s="2"/>
       <c r="D43" t="s" s="2">
@@ -7658,13 +7653,13 @@
         <v>50</v>
       </c>
       <c r="K43" t="s" s="2">
+        <v>363</v>
+      </c>
+      <c r="L43" t="s" s="2">
         <v>364</v>
       </c>
-      <c r="L43" t="s" s="2">
+      <c r="M43" t="s" s="2">
         <v>365</v>
-      </c>
-      <c r="M43" t="s" s="2">
-        <v>366</v>
       </c>
       <c r="N43" s="2"/>
       <c r="O43" s="2"/>
@@ -7715,7 +7710,7 @@
         <v>35</v>
       </c>
       <c r="AF43" t="s" s="2">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="AG43" t="s" s="2">
         <v>49</v>
@@ -7733,22 +7728,22 @@
         <v>35</v>
       </c>
       <c r="AL43" t="s" s="2">
+        <v>366</v>
+      </c>
+      <c r="AM43" t="s" s="2">
+        <v>358</v>
+      </c>
+      <c r="AN43" t="s" s="2">
         <v>367</v>
       </c>
-      <c r="AM43" t="s" s="2">
-        <v>359</v>
-      </c>
-      <c r="AN43" t="s" s="2">
+      <c r="AO43" t="s" s="2">
+        <v>35</v>
+      </c>
+      <c r="AP43" t="s" s="2">
         <v>368</v>
       </c>
-      <c r="AO43" t="s" s="2">
-        <v>35</v>
-      </c>
-      <c r="AP43" t="s" s="2">
+      <c r="AQ43" t="s" s="2">
         <v>369</v>
-      </c>
-      <c r="AQ43" t="s" s="2">
-        <v>370</v>
       </c>
       <c r="AR43" t="s" s="2">
         <v>35</v>
@@ -7759,10 +7754,10 @@
     </row>
     <row r="44" hidden="true">
       <c r="A44" t="s" s="2">
-        <v>371</v>
+        <v>370</v>
       </c>
       <c r="B44" t="s" s="2">
-        <v>371</v>
+        <v>370</v>
       </c>
       <c r="C44" s="2"/>
       <c r="D44" t="s" s="2">
@@ -7886,10 +7881,10 @@
     </row>
     <row r="45" hidden="true">
       <c r="A45" t="s" s="2">
-        <v>372</v>
+        <v>371</v>
       </c>
       <c r="B45" t="s" s="2">
-        <v>372</v>
+        <v>371</v>
       </c>
       <c r="C45" s="2"/>
       <c r="D45" t="s" s="2">
@@ -8015,10 +8010,10 @@
     </row>
     <row r="46" hidden="true">
       <c r="A46" t="s" s="2">
-        <v>373</v>
+        <v>372</v>
       </c>
       <c r="B46" t="s" s="2">
-        <v>373</v>
+        <v>372</v>
       </c>
       <c r="C46" s="2"/>
       <c r="D46" t="s" s="2">
@@ -8044,14 +8039,14 @@
         <v>127</v>
       </c>
       <c r="L46" t="s" s="2">
+        <v>373</v>
+      </c>
+      <c r="M46" t="s" s="2">
         <v>374</v>
-      </c>
-      <c r="M46" t="s" s="2">
-        <v>375</v>
       </c>
       <c r="N46" s="2"/>
       <c r="O46" t="s" s="2">
-        <v>376</v>
+        <v>375</v>
       </c>
       <c r="P46" t="s" s="2">
         <v>35</v>
@@ -8064,7 +8059,7 @@
         <v>35</v>
       </c>
       <c r="T46" t="s" s="2">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="U46" t="s" s="2">
         <v>35</v>
@@ -8079,28 +8074,28 @@
         <v>193</v>
       </c>
       <c r="Y46" t="s" s="2">
+        <v>377</v>
+      </c>
+      <c r="Z46" t="s" s="2">
         <v>378</v>
       </c>
-      <c r="Z46" t="s" s="2">
+      <c r="AA46" t="s" s="2">
+        <v>35</v>
+      </c>
+      <c r="AB46" t="s" s="2">
+        <v>35</v>
+      </c>
+      <c r="AC46" t="s" s="2">
+        <v>35</v>
+      </c>
+      <c r="AD46" t="s" s="2">
+        <v>35</v>
+      </c>
+      <c r="AE46" t="s" s="2">
+        <v>35</v>
+      </c>
+      <c r="AF46" t="s" s="2">
         <v>379</v>
-      </c>
-      <c r="AA46" t="s" s="2">
-        <v>35</v>
-      </c>
-      <c r="AB46" t="s" s="2">
-        <v>35</v>
-      </c>
-      <c r="AC46" t="s" s="2">
-        <v>35</v>
-      </c>
-      <c r="AD46" t="s" s="2">
-        <v>35</v>
-      </c>
-      <c r="AE46" t="s" s="2">
-        <v>35</v>
-      </c>
-      <c r="AF46" t="s" s="2">
-        <v>380</v>
       </c>
       <c r="AG46" t="s" s="2">
         <v>36</v>
@@ -8121,22 +8116,22 @@
         <v>35</v>
       </c>
       <c r="AM46" t="s" s="2">
+        <v>380</v>
+      </c>
+      <c r="AN46" t="s" s="2">
+        <v>35</v>
+      </c>
+      <c r="AO46" t="s" s="2">
+        <v>35</v>
+      </c>
+      <c r="AP46" t="s" s="2">
         <v>381</v>
       </c>
-      <c r="AN46" t="s" s="2">
-        <v>35</v>
-      </c>
-      <c r="AO46" t="s" s="2">
-        <v>35</v>
-      </c>
-      <c r="AP46" t="s" s="2">
+      <c r="AQ46" t="s" s="2">
+        <v>35</v>
+      </c>
+      <c r="AR46" t="s" s="2">
         <v>382</v>
-      </c>
-      <c r="AQ46" t="s" s="2">
-        <v>35</v>
-      </c>
-      <c r="AR46" t="s" s="2">
-        <v>383</v>
       </c>
       <c r="AS46" t="s" s="2">
         <v>35</v>
@@ -8144,10 +8139,10 @@
     </row>
     <row r="47" hidden="true">
       <c r="A47" t="s" s="2">
-        <v>384</v>
+        <v>383</v>
       </c>
       <c r="B47" t="s" s="2">
-        <v>384</v>
+        <v>383</v>
       </c>
       <c r="C47" s="2"/>
       <c r="D47" t="s" s="2">
@@ -8173,14 +8168,14 @@
         <v>127</v>
       </c>
       <c r="L47" t="s" s="2">
+        <v>384</v>
+      </c>
+      <c r="M47" t="s" s="2">
         <v>385</v>
-      </c>
-      <c r="M47" t="s" s="2">
-        <v>386</v>
       </c>
       <c r="N47" s="2"/>
       <c r="O47" t="s" s="2">
-        <v>387</v>
+        <v>386</v>
       </c>
       <c r="P47" t="s" s="2">
         <v>35</v>
@@ -8193,7 +8188,7 @@
         <v>35</v>
       </c>
       <c r="T47" t="s" s="2">
-        <v>388</v>
+        <v>387</v>
       </c>
       <c r="U47" t="s" s="2">
         <v>35</v>
@@ -8229,7 +8224,7 @@
         <v>35</v>
       </c>
       <c r="AF47" t="s" s="2">
-        <v>389</v>
+        <v>388</v>
       </c>
       <c r="AG47" t="s" s="2">
         <v>36</v>
@@ -8250,33 +8245,33 @@
         <v>35</v>
       </c>
       <c r="AM47" t="s" s="2">
+        <v>389</v>
+      </c>
+      <c r="AN47" t="s" s="2">
+        <v>35</v>
+      </c>
+      <c r="AO47" t="s" s="2">
+        <v>35</v>
+      </c>
+      <c r="AP47" t="s" s="2">
+        <v>35</v>
+      </c>
+      <c r="AQ47" t="s" s="2">
+        <v>35</v>
+      </c>
+      <c r="AR47" t="s" s="2">
         <v>390</v>
       </c>
-      <c r="AN47" t="s" s="2">
-        <v>35</v>
-      </c>
-      <c r="AO47" t="s" s="2">
-        <v>35</v>
-      </c>
-      <c r="AP47" t="s" s="2">
-        <v>35</v>
-      </c>
-      <c r="AQ47" t="s" s="2">
-        <v>35</v>
-      </c>
-      <c r="AR47" t="s" s="2">
+      <c r="AS47" t="s" s="2">
         <v>391</v>
-      </c>
-      <c r="AS47" t="s" s="2">
-        <v>392</v>
       </c>
     </row>
     <row r="48" hidden="true">
       <c r="A48" t="s" s="2">
-        <v>393</v>
+        <v>392</v>
       </c>
       <c r="B48" t="s" s="2">
-        <v>393</v>
+        <v>392</v>
       </c>
       <c r="C48" s="2"/>
       <c r="D48" t="s" s="2">
@@ -8299,19 +8294,19 @@
         <v>35</v>
       </c>
       <c r="K48" t="s" s="2">
+        <v>393</v>
+      </c>
+      <c r="L48" t="s" s="2">
         <v>394</v>
       </c>
-      <c r="L48" t="s" s="2">
+      <c r="M48" t="s" s="2">
         <v>395</v>
       </c>
-      <c r="M48" t="s" s="2">
+      <c r="N48" t="s" s="2">
         <v>396</v>
       </c>
-      <c r="N48" t="s" s="2">
+      <c r="O48" t="s" s="2">
         <v>397</v>
-      </c>
-      <c r="O48" t="s" s="2">
-        <v>398</v>
       </c>
       <c r="P48" t="s" s="2">
         <v>35</v>
@@ -8360,7 +8355,7 @@
         <v>35</v>
       </c>
       <c r="AF48" t="s" s="2">
-        <v>399</v>
+        <v>398</v>
       </c>
       <c r="AG48" t="s" s="2">
         <v>36</v>
@@ -8381,16 +8376,16 @@
         <v>35</v>
       </c>
       <c r="AM48" t="s" s="2">
+        <v>399</v>
+      </c>
+      <c r="AN48" t="s" s="2">
+        <v>35</v>
+      </c>
+      <c r="AO48" t="s" s="2">
+        <v>35</v>
+      </c>
+      <c r="AP48" t="s" s="2">
         <v>400</v>
-      </c>
-      <c r="AN48" t="s" s="2">
-        <v>35</v>
-      </c>
-      <c r="AO48" t="s" s="2">
-        <v>35</v>
-      </c>
-      <c r="AP48" t="s" s="2">
-        <v>401</v>
       </c>
       <c r="AQ48" t="s" s="2">
         <v>35</v>
@@ -8404,10 +8399,10 @@
     </row>
     <row r="49" hidden="true">
       <c r="A49" t="s" s="2">
-        <v>402</v>
+        <v>401</v>
       </c>
       <c r="B49" t="s" s="2">
-        <v>402</v>
+        <v>401</v>
       </c>
       <c r="C49" s="2"/>
       <c r="D49" t="s" s="2">
@@ -8430,19 +8425,19 @@
         <v>50</v>
       </c>
       <c r="K49" t="s" s="2">
+        <v>402</v>
+      </c>
+      <c r="L49" t="s" s="2">
         <v>403</v>
       </c>
-      <c r="L49" t="s" s="2">
+      <c r="M49" t="s" s="2">
         <v>404</v>
       </c>
-      <c r="M49" t="s" s="2">
+      <c r="N49" t="s" s="2">
         <v>405</v>
       </c>
-      <c r="N49" t="s" s="2">
+      <c r="O49" t="s" s="2">
         <v>406</v>
-      </c>
-      <c r="O49" t="s" s="2">
-        <v>407</v>
       </c>
       <c r="P49" t="s" s="2">
         <v>35</v>
@@ -8455,90 +8450,90 @@
         <v>35</v>
       </c>
       <c r="T49" t="s" s="2">
+        <v>407</v>
+      </c>
+      <c r="U49" t="s" s="2">
+        <v>35</v>
+      </c>
+      <c r="V49" t="s" s="2">
+        <v>35</v>
+      </c>
+      <c r="W49" t="s" s="2">
+        <v>35</v>
+      </c>
+      <c r="X49" t="s" s="2">
+        <v>35</v>
+      </c>
+      <c r="Y49" t="s" s="2">
+        <v>35</v>
+      </c>
+      <c r="Z49" t="s" s="2">
+        <v>35</v>
+      </c>
+      <c r="AA49" t="s" s="2">
+        <v>35</v>
+      </c>
+      <c r="AB49" t="s" s="2">
+        <v>35</v>
+      </c>
+      <c r="AC49" t="s" s="2">
+        <v>35</v>
+      </c>
+      <c r="AD49" t="s" s="2">
+        <v>35</v>
+      </c>
+      <c r="AE49" t="s" s="2">
+        <v>35</v>
+      </c>
+      <c r="AF49" t="s" s="2">
         <v>408</v>
       </c>
-      <c r="U49" t="s" s="2">
-        <v>35</v>
-      </c>
-      <c r="V49" t="s" s="2">
-        <v>35</v>
-      </c>
-      <c r="W49" t="s" s="2">
-        <v>35</v>
-      </c>
-      <c r="X49" t="s" s="2">
-        <v>35</v>
-      </c>
-      <c r="Y49" t="s" s="2">
-        <v>35</v>
-      </c>
-      <c r="Z49" t="s" s="2">
-        <v>35</v>
-      </c>
-      <c r="AA49" t="s" s="2">
-        <v>35</v>
-      </c>
-      <c r="AB49" t="s" s="2">
-        <v>35</v>
-      </c>
-      <c r="AC49" t="s" s="2">
-        <v>35</v>
-      </c>
-      <c r="AD49" t="s" s="2">
-        <v>35</v>
-      </c>
-      <c r="AE49" t="s" s="2">
-        <v>35</v>
-      </c>
-      <c r="AF49" t="s" s="2">
+      <c r="AG49" t="s" s="2">
+        <v>36</v>
+      </c>
+      <c r="AH49" t="s" s="2">
+        <v>49</v>
+      </c>
+      <c r="AI49" t="s" s="2">
+        <v>35</v>
+      </c>
+      <c r="AJ49" t="s" s="2">
         <v>409</v>
       </c>
-      <c r="AG49" t="s" s="2">
-        <v>36</v>
-      </c>
-      <c r="AH49" t="s" s="2">
-        <v>49</v>
-      </c>
-      <c r="AI49" t="s" s="2">
-        <v>35</v>
-      </c>
-      <c r="AJ49" t="s" s="2">
+      <c r="AK49" t="s" s="2">
+        <v>35</v>
+      </c>
+      <c r="AL49" t="s" s="2">
+        <v>35</v>
+      </c>
+      <c r="AM49" t="s" s="2">
         <v>410</v>
       </c>
-      <c r="AK49" t="s" s="2">
-        <v>35</v>
-      </c>
-      <c r="AL49" t="s" s="2">
-        <v>35</v>
-      </c>
-      <c r="AM49" t="s" s="2">
+      <c r="AN49" t="s" s="2">
+        <v>35</v>
+      </c>
+      <c r="AO49" t="s" s="2">
+        <v>35</v>
+      </c>
+      <c r="AP49" t="s" s="2">
         <v>411</v>
       </c>
-      <c r="AN49" t="s" s="2">
-        <v>35</v>
-      </c>
-      <c r="AO49" t="s" s="2">
-        <v>35</v>
-      </c>
-      <c r="AP49" t="s" s="2">
+      <c r="AQ49" t="s" s="2">
+        <v>35</v>
+      </c>
+      <c r="AR49" t="s" s="2">
         <v>412</v>
       </c>
-      <c r="AQ49" t="s" s="2">
-        <v>35</v>
-      </c>
-      <c r="AR49" t="s" s="2">
+      <c r="AS49" t="s" s="2">
         <v>413</v>
-      </c>
-      <c r="AS49" t="s" s="2">
-        <v>414</v>
       </c>
     </row>
     <row r="50" hidden="true">
       <c r="A50" t="s" s="2">
-        <v>415</v>
+        <v>414</v>
       </c>
       <c r="B50" t="s" s="2">
-        <v>415</v>
+        <v>414</v>
       </c>
       <c r="C50" s="2"/>
       <c r="D50" t="s" s="2">
@@ -8561,19 +8556,19 @@
         <v>50</v>
       </c>
       <c r="K50" t="s" s="2">
+        <v>415</v>
+      </c>
+      <c r="L50" t="s" s="2">
         <v>416</v>
       </c>
-      <c r="L50" t="s" s="2">
+      <c r="M50" t="s" s="2">
         <v>417</v>
       </c>
-      <c r="M50" t="s" s="2">
+      <c r="N50" t="s" s="2">
         <v>418</v>
       </c>
-      <c r="N50" t="s" s="2">
+      <c r="O50" t="s" s="2">
         <v>419</v>
-      </c>
-      <c r="O50" t="s" s="2">
-        <v>420</v>
       </c>
       <c r="P50" t="s" s="2">
         <v>35</v>
@@ -8622,7 +8617,7 @@
         <v>35</v>
       </c>
       <c r="AF50" t="s" s="2">
-        <v>421</v>
+        <v>420</v>
       </c>
       <c r="AG50" t="s" s="2">
         <v>36</v>
@@ -8643,22 +8638,22 @@
         <v>35</v>
       </c>
       <c r="AM50" t="s" s="2">
+        <v>421</v>
+      </c>
+      <c r="AN50" t="s" s="2">
+        <v>35</v>
+      </c>
+      <c r="AO50" t="s" s="2">
+        <v>35</v>
+      </c>
+      <c r="AP50" t="s" s="2">
+        <v>35</v>
+      </c>
+      <c r="AQ50" t="s" s="2">
+        <v>35</v>
+      </c>
+      <c r="AR50" t="s" s="2">
         <v>422</v>
-      </c>
-      <c r="AN50" t="s" s="2">
-        <v>35</v>
-      </c>
-      <c r="AO50" t="s" s="2">
-        <v>35</v>
-      </c>
-      <c r="AP50" t="s" s="2">
-        <v>35</v>
-      </c>
-      <c r="AQ50" t="s" s="2">
-        <v>35</v>
-      </c>
-      <c r="AR50" t="s" s="2">
-        <v>423</v>
       </c>
       <c r="AS50" t="s" s="2">
         <v>35</v>
@@ -8666,10 +8661,10 @@
     </row>
     <row r="51" hidden="true">
       <c r="A51" t="s" s="2">
-        <v>424</v>
+        <v>423</v>
       </c>
       <c r="B51" t="s" s="2">
-        <v>424</v>
+        <v>423</v>
       </c>
       <c r="C51" s="2"/>
       <c r="D51" t="s" s="2">
@@ -8692,19 +8687,19 @@
         <v>50</v>
       </c>
       <c r="K51" t="s" s="2">
-        <v>394</v>
+        <v>393</v>
       </c>
       <c r="L51" t="s" s="2">
+        <v>424</v>
+      </c>
+      <c r="M51" t="s" s="2">
         <v>425</v>
       </c>
-      <c r="M51" t="s" s="2">
+      <c r="N51" t="s" s="2">
         <v>426</v>
       </c>
-      <c r="N51" t="s" s="2">
+      <c r="O51" t="s" s="2">
         <v>427</v>
-      </c>
-      <c r="O51" t="s" s="2">
-        <v>428</v>
       </c>
       <c r="P51" t="s" s="2">
         <v>35</v>
@@ -8753,7 +8748,7 @@
         <v>35</v>
       </c>
       <c r="AF51" t="s" s="2">
-        <v>429</v>
+        <v>428</v>
       </c>
       <c r="AG51" t="s" s="2">
         <v>36</v>
@@ -8774,22 +8769,22 @@
         <v>35</v>
       </c>
       <c r="AM51" t="s" s="2">
+        <v>429</v>
+      </c>
+      <c r="AN51" t="s" s="2">
+        <v>35</v>
+      </c>
+      <c r="AO51" t="s" s="2">
+        <v>35</v>
+      </c>
+      <c r="AP51" t="s" s="2">
+        <v>35</v>
+      </c>
+      <c r="AQ51" t="s" s="2">
+        <v>35</v>
+      </c>
+      <c r="AR51" t="s" s="2">
         <v>430</v>
-      </c>
-      <c r="AN51" t="s" s="2">
-        <v>35</v>
-      </c>
-      <c r="AO51" t="s" s="2">
-        <v>35</v>
-      </c>
-      <c r="AP51" t="s" s="2">
-        <v>35</v>
-      </c>
-      <c r="AQ51" t="s" s="2">
-        <v>35</v>
-      </c>
-      <c r="AR51" t="s" s="2">
-        <v>431</v>
       </c>
       <c r="AS51" t="s" s="2">
         <v>35</v>
@@ -8797,10 +8792,10 @@
     </row>
     <row r="52" hidden="true">
       <c r="A52" t="s" s="2">
-        <v>432</v>
+        <v>431</v>
       </c>
       <c r="B52" t="s" s="2">
-        <v>432</v>
+        <v>431</v>
       </c>
       <c r="C52" s="2"/>
       <c r="D52" t="s" s="2">
@@ -8826,14 +8821,14 @@
         <v>62</v>
       </c>
       <c r="L52" t="s" s="2">
+        <v>432</v>
+      </c>
+      <c r="M52" t="s" s="2">
         <v>433</v>
-      </c>
-      <c r="M52" t="s" s="2">
-        <v>434</v>
       </c>
       <c r="N52" s="2"/>
       <c r="O52" t="s" s="2">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="P52" t="s" s="2">
         <v>35</v>
@@ -8846,43 +8841,43 @@
         <v>35</v>
       </c>
       <c r="T52" t="s" s="2">
+        <v>435</v>
+      </c>
+      <c r="U52" t="s" s="2">
+        <v>35</v>
+      </c>
+      <c r="V52" t="s" s="2">
+        <v>35</v>
+      </c>
+      <c r="W52" t="s" s="2">
+        <v>35</v>
+      </c>
+      <c r="X52" t="s" s="2">
+        <v>35</v>
+      </c>
+      <c r="Y52" t="s" s="2">
+        <v>35</v>
+      </c>
+      <c r="Z52" t="s" s="2">
+        <v>35</v>
+      </c>
+      <c r="AA52" t="s" s="2">
+        <v>35</v>
+      </c>
+      <c r="AB52" t="s" s="2">
+        <v>35</v>
+      </c>
+      <c r="AC52" t="s" s="2">
+        <v>35</v>
+      </c>
+      <c r="AD52" t="s" s="2">
+        <v>35</v>
+      </c>
+      <c r="AE52" t="s" s="2">
+        <v>35</v>
+      </c>
+      <c r="AF52" t="s" s="2">
         <v>436</v>
-      </c>
-      <c r="U52" t="s" s="2">
-        <v>35</v>
-      </c>
-      <c r="V52" t="s" s="2">
-        <v>35</v>
-      </c>
-      <c r="W52" t="s" s="2">
-        <v>35</v>
-      </c>
-      <c r="X52" t="s" s="2">
-        <v>35</v>
-      </c>
-      <c r="Y52" t="s" s="2">
-        <v>35</v>
-      </c>
-      <c r="Z52" t="s" s="2">
-        <v>35</v>
-      </c>
-      <c r="AA52" t="s" s="2">
-        <v>35</v>
-      </c>
-      <c r="AB52" t="s" s="2">
-        <v>35</v>
-      </c>
-      <c r="AC52" t="s" s="2">
-        <v>35</v>
-      </c>
-      <c r="AD52" t="s" s="2">
-        <v>35</v>
-      </c>
-      <c r="AE52" t="s" s="2">
-        <v>35</v>
-      </c>
-      <c r="AF52" t="s" s="2">
-        <v>437</v>
       </c>
       <c r="AG52" t="s" s="2">
         <v>36</v>
@@ -8903,33 +8898,33 @@
         <v>35</v>
       </c>
       <c r="AM52" t="s" s="2">
+        <v>437</v>
+      </c>
+      <c r="AN52" t="s" s="2">
+        <v>35</v>
+      </c>
+      <c r="AO52" t="s" s="2">
+        <v>35</v>
+      </c>
+      <c r="AP52" t="s" s="2">
+        <v>35</v>
+      </c>
+      <c r="AQ52" t="s" s="2">
+        <v>35</v>
+      </c>
+      <c r="AR52" t="s" s="2">
         <v>438</v>
       </c>
-      <c r="AN52" t="s" s="2">
-        <v>35</v>
-      </c>
-      <c r="AO52" t="s" s="2">
-        <v>35</v>
-      </c>
-      <c r="AP52" t="s" s="2">
-        <v>35</v>
-      </c>
-      <c r="AQ52" t="s" s="2">
-        <v>35</v>
-      </c>
-      <c r="AR52" t="s" s="2">
+      <c r="AS52" t="s" s="2">
         <v>439</v>
-      </c>
-      <c r="AS52" t="s" s="2">
-        <v>440</v>
       </c>
     </row>
     <row r="53" hidden="true">
       <c r="A53" t="s" s="2">
-        <v>441</v>
+        <v>440</v>
       </c>
       <c r="B53" t="s" s="2">
-        <v>441</v>
+        <v>440</v>
       </c>
       <c r="C53" s="2"/>
       <c r="D53" t="s" s="2">
@@ -8952,17 +8947,17 @@
         <v>50</v>
       </c>
       <c r="K53" t="s" s="2">
+        <v>441</v>
+      </c>
+      <c r="L53" t="s" s="2">
         <v>442</v>
       </c>
-      <c r="L53" t="s" s="2">
+      <c r="M53" t="s" s="2">
         <v>443</v>
-      </c>
-      <c r="M53" t="s" s="2">
-        <v>444</v>
       </c>
       <c r="N53" s="2"/>
       <c r="O53" t="s" s="2">
-        <v>445</v>
+        <v>444</v>
       </c>
       <c r="P53" t="s" s="2">
         <v>35</v>
@@ -9011,7 +9006,7 @@
         <v>35</v>
       </c>
       <c r="AF53" t="s" s="2">
-        <v>446</v>
+        <v>445</v>
       </c>
       <c r="AG53" t="s" s="2">
         <v>36</v>
@@ -9032,7 +9027,7 @@
         <v>35</v>
       </c>
       <c r="AM53" t="s" s="2">
-        <v>422</v>
+        <v>421</v>
       </c>
       <c r="AN53" t="s" s="2">
         <v>35</v>
@@ -9047,18 +9042,18 @@
         <v>35</v>
       </c>
       <c r="AR53" t="s" s="2">
+        <v>446</v>
+      </c>
+      <c r="AS53" t="s" s="2">
         <v>447</v>
-      </c>
-      <c r="AS53" t="s" s="2">
-        <v>448</v>
       </c>
     </row>
     <row r="54" hidden="true">
       <c r="A54" t="s" s="2">
-        <v>449</v>
+        <v>448</v>
       </c>
       <c r="B54" t="s" s="2">
-        <v>449</v>
+        <v>448</v>
       </c>
       <c r="C54" s="2"/>
       <c r="D54" t="s" s="2">
@@ -9084,13 +9079,13 @@
         <v>105</v>
       </c>
       <c r="L54" t="s" s="2">
+        <v>449</v>
+      </c>
+      <c r="M54" t="s" s="2">
         <v>450</v>
       </c>
-      <c r="M54" t="s" s="2">
+      <c r="N54" t="s" s="2">
         <v>451</v>
-      </c>
-      <c r="N54" t="s" s="2">
-        <v>452</v>
       </c>
       <c r="O54" s="2"/>
       <c r="P54" t="s" s="2">
@@ -9119,75 +9114,75 @@
         <v>131</v>
       </c>
       <c r="Y54" t="s" s="2">
+        <v>452</v>
+      </c>
+      <c r="Z54" t="s" s="2">
         <v>453</v>
       </c>
-      <c r="Z54" t="s" s="2">
+      <c r="AA54" t="s" s="2">
+        <v>35</v>
+      </c>
+      <c r="AB54" t="s" s="2">
+        <v>35</v>
+      </c>
+      <c r="AC54" t="s" s="2">
+        <v>35</v>
+      </c>
+      <c r="AD54" t="s" s="2">
+        <v>35</v>
+      </c>
+      <c r="AE54" t="s" s="2">
+        <v>35</v>
+      </c>
+      <c r="AF54" t="s" s="2">
+        <v>448</v>
+      </c>
+      <c r="AG54" t="s" s="2">
+        <v>36</v>
+      </c>
+      <c r="AH54" t="s" s="2">
+        <v>49</v>
+      </c>
+      <c r="AI54" t="s" s="2">
+        <v>35</v>
+      </c>
+      <c r="AJ54" t="s" s="2">
         <v>454</v>
       </c>
-      <c r="AA54" t="s" s="2">
-        <v>35</v>
-      </c>
-      <c r="AB54" t="s" s="2">
-        <v>35</v>
-      </c>
-      <c r="AC54" t="s" s="2">
-        <v>35</v>
-      </c>
-      <c r="AD54" t="s" s="2">
-        <v>35</v>
-      </c>
-      <c r="AE54" t="s" s="2">
-        <v>35</v>
-      </c>
-      <c r="AF54" t="s" s="2">
-        <v>449</v>
-      </c>
-      <c r="AG54" t="s" s="2">
-        <v>36</v>
-      </c>
-      <c r="AH54" t="s" s="2">
-        <v>49</v>
-      </c>
-      <c r="AI54" t="s" s="2">
-        <v>35</v>
-      </c>
-      <c r="AJ54" t="s" s="2">
+      <c r="AK54" t="s" s="2">
+        <v>35</v>
+      </c>
+      <c r="AL54" t="s" s="2">
         <v>455</v>
       </c>
-      <c r="AK54" t="s" s="2">
-        <v>35</v>
-      </c>
-      <c r="AL54" t="s" s="2">
+      <c r="AM54" t="s" s="2">
+        <v>358</v>
+      </c>
+      <c r="AN54" t="s" s="2">
         <v>456</v>
       </c>
-      <c r="AM54" t="s" s="2">
-        <v>359</v>
-      </c>
-      <c r="AN54" t="s" s="2">
+      <c r="AO54" t="s" s="2">
+        <v>35</v>
+      </c>
+      <c r="AP54" t="s" s="2">
+        <v>35</v>
+      </c>
+      <c r="AQ54" t="s" s="2">
         <v>457</v>
       </c>
-      <c r="AO54" t="s" s="2">
-        <v>35</v>
-      </c>
-      <c r="AP54" t="s" s="2">
-        <v>35</v>
-      </c>
-      <c r="AQ54" t="s" s="2">
+      <c r="AR54" t="s" s="2">
+        <v>457</v>
+      </c>
+      <c r="AS54" t="s" s="2">
         <v>458</v>
-      </c>
-      <c r="AR54" t="s" s="2">
-        <v>458</v>
-      </c>
-      <c r="AS54" t="s" s="2">
-        <v>459</v>
       </c>
     </row>
     <row r="55" hidden="true">
       <c r="A55" t="s" s="2">
-        <v>460</v>
+        <v>459</v>
       </c>
       <c r="B55" t="s" s="2">
-        <v>460</v>
+        <v>459</v>
       </c>
       <c r="C55" s="2"/>
       <c r="D55" t="s" s="2">
@@ -9210,16 +9205,16 @@
         <v>50</v>
       </c>
       <c r="K55" t="s" s="2">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="L55" t="s" s="2">
+        <v>460</v>
+      </c>
+      <c r="M55" t="s" s="2">
         <v>461</v>
       </c>
-      <c r="M55" t="s" s="2">
+      <c r="N55" t="s" s="2">
         <v>462</v>
-      </c>
-      <c r="N55" t="s" s="2">
-        <v>463</v>
       </c>
       <c r="O55" s="2"/>
       <c r="P55" t="s" s="2">
@@ -9269,7 +9264,7 @@
         <v>35</v>
       </c>
       <c r="AF55" t="s" s="2">
-        <v>460</v>
+        <v>459</v>
       </c>
       <c r="AG55" t="s" s="2">
         <v>36</v>
@@ -9290,7 +9285,7 @@
         <v>35</v>
       </c>
       <c r="AM55" t="s" s="2">
-        <v>464</v>
+        <v>463</v>
       </c>
       <c r="AN55" t="s" s="2">
         <v>35</v>
@@ -9313,10 +9308,10 @@
     </row>
     <row r="56" hidden="true">
       <c r="A56" t="s" s="2">
-        <v>465</v>
+        <v>464</v>
       </c>
       <c r="B56" t="s" s="2">
-        <v>465</v>
+        <v>464</v>
       </c>
       <c r="C56" s="2"/>
       <c r="D56" t="s" s="2">
@@ -9440,10 +9435,10 @@
     </row>
     <row r="57" hidden="true">
       <c r="A57" t="s" s="2">
-        <v>466</v>
+        <v>465</v>
       </c>
       <c r="B57" t="s" s="2">
-        <v>466</v>
+        <v>465</v>
       </c>
       <c r="C57" s="2"/>
       <c r="D57" t="s" s="2">
@@ -9569,14 +9564,14 @@
     </row>
     <row r="58" hidden="true">
       <c r="A58" t="s" s="2">
-        <v>467</v>
+        <v>466</v>
       </c>
       <c r="B58" t="s" s="2">
-        <v>467</v>
+        <v>466</v>
       </c>
       <c r="C58" s="2"/>
       <c r="D58" t="s" s="2">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="E58" s="2"/>
       <c r="F58" t="s" s="2">
@@ -9598,16 +9593,16 @@
         <v>69</v>
       </c>
       <c r="L58" t="s" s="2">
+        <v>308</v>
+      </c>
+      <c r="M58" t="s" s="2">
         <v>309</v>
-      </c>
-      <c r="M58" t="s" s="2">
-        <v>310</v>
       </c>
       <c r="N58" t="s" s="2">
         <v>72</v>
       </c>
       <c r="O58" t="s" s="2">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="P58" t="s" s="2">
         <v>35</v>
@@ -9656,7 +9651,7 @@
         <v>35</v>
       </c>
       <c r="AF58" t="s" s="2">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="AG58" t="s" s="2">
         <v>36</v>
@@ -9700,10 +9695,10 @@
     </row>
     <row r="59" hidden="true">
       <c r="A59" t="s" s="2">
-        <v>468</v>
+        <v>467</v>
       </c>
       <c r="B59" t="s" s="2">
-        <v>468</v>
+        <v>467</v>
       </c>
       <c r="C59" s="2"/>
       <c r="D59" t="s" s="2">
@@ -9726,13 +9721,13 @@
         <v>35</v>
       </c>
       <c r="K59" t="s" s="2">
+        <v>468</v>
+      </c>
+      <c r="L59" t="s" s="2">
         <v>469</v>
       </c>
-      <c r="L59" t="s" s="2">
+      <c r="M59" t="s" s="2">
         <v>470</v>
-      </c>
-      <c r="M59" t="s" s="2">
-        <v>471</v>
       </c>
       <c r="N59" s="2"/>
       <c r="O59" s="2"/>
@@ -9783,7 +9778,7 @@
         <v>35</v>
       </c>
       <c r="AF59" t="s" s="2">
-        <v>468</v>
+        <v>467</v>
       </c>
       <c r="AG59" t="s" s="2">
         <v>36</v>
@@ -9798,28 +9793,28 @@
         <v>83</v>
       </c>
       <c r="AK59" t="s" s="2">
+        <v>471</v>
+      </c>
+      <c r="AL59" t="s" s="2">
         <v>472</v>
       </c>
-      <c r="AL59" t="s" s="2">
+      <c r="AM59" t="s" s="2">
         <v>473</v>
       </c>
-      <c r="AM59" t="s" s="2">
+      <c r="AN59" t="s" s="2">
+        <v>35</v>
+      </c>
+      <c r="AO59" t="s" s="2">
         <v>474</v>
       </c>
-      <c r="AN59" t="s" s="2">
-        <v>35</v>
-      </c>
-      <c r="AO59" t="s" s="2">
+      <c r="AP59" t="s" s="2">
+        <v>35</v>
+      </c>
+      <c r="AQ59" t="s" s="2">
+        <v>35</v>
+      </c>
+      <c r="AR59" t="s" s="2">
         <v>475</v>
-      </c>
-      <c r="AP59" t="s" s="2">
-        <v>35</v>
-      </c>
-      <c r="AQ59" t="s" s="2">
-        <v>35</v>
-      </c>
-      <c r="AR59" t="s" s="2">
-        <v>476</v>
       </c>
       <c r="AS59" t="s" s="2">
         <v>35</v>
@@ -9827,10 +9822,10 @@
     </row>
     <row r="60" hidden="true">
       <c r="A60" t="s" s="2">
-        <v>477</v>
+        <v>476</v>
       </c>
       <c r="B60" t="s" s="2">
-        <v>477</v>
+        <v>476</v>
       </c>
       <c r="C60" s="2"/>
       <c r="D60" t="s" s="2">
@@ -9856,13 +9851,13 @@
         <v>210</v>
       </c>
       <c r="L60" t="s" s="2">
+        <v>477</v>
+      </c>
+      <c r="M60" t="s" s="2">
         <v>478</v>
       </c>
-      <c r="M60" t="s" s="2">
+      <c r="N60" t="s" s="2">
         <v>479</v>
-      </c>
-      <c r="N60" t="s" s="2">
-        <v>480</v>
       </c>
       <c r="O60" s="2"/>
       <c r="P60" t="s" s="2">
@@ -9891,11 +9886,11 @@
         <v>117</v>
       </c>
       <c r="Y60" t="s" s="2">
+        <v>480</v>
+      </c>
+      <c r="Z60" t="s" s="2">
         <v>481</v>
       </c>
-      <c r="Z60" t="s" s="2">
-        <v>482</v>
-      </c>
       <c r="AA60" t="s" s="2">
         <v>35</v>
       </c>
@@ -9912,7 +9907,7 @@
         <v>35</v>
       </c>
       <c r="AF60" t="s" s="2">
-        <v>477</v>
+        <v>476</v>
       </c>
       <c r="AG60" t="s" s="2">
         <v>36</v>
@@ -9924,42 +9919,42 @@
         <v>35</v>
       </c>
       <c r="AJ60" t="s" s="2">
+        <v>482</v>
+      </c>
+      <c r="AK60" t="s" s="2">
+        <v>35</v>
+      </c>
+      <c r="AL60" t="s" s="2">
         <v>483</v>
       </c>
-      <c r="AK60" t="s" s="2">
-        <v>35</v>
-      </c>
-      <c r="AL60" t="s" s="2">
+      <c r="AM60" t="s" s="2">
         <v>484</v>
       </c>
-      <c r="AM60" t="s" s="2">
+      <c r="AN60" t="s" s="2">
+        <v>35</v>
+      </c>
+      <c r="AO60" t="s" s="2">
+        <v>35</v>
+      </c>
+      <c r="AP60" t="s" s="2">
+        <v>35</v>
+      </c>
+      <c r="AQ60" t="s" s="2">
         <v>485</v>
       </c>
-      <c r="AN60" t="s" s="2">
-        <v>35</v>
-      </c>
-      <c r="AO60" t="s" s="2">
-        <v>35</v>
-      </c>
-      <c r="AP60" t="s" s="2">
-        <v>35</v>
-      </c>
-      <c r="AQ60" t="s" s="2">
+      <c r="AR60" t="s" s="2">
+        <v>485</v>
+      </c>
+      <c r="AS60" t="s" s="2">
         <v>486</v>
-      </c>
-      <c r="AR60" t="s" s="2">
-        <v>486</v>
-      </c>
-      <c r="AS60" t="s" s="2">
-        <v>487</v>
       </c>
     </row>
     <row r="61" hidden="true">
       <c r="A61" t="s" s="2">
-        <v>488</v>
+        <v>487</v>
       </c>
       <c r="B61" t="s" s="2">
-        <v>488</v>
+        <v>487</v>
       </c>
       <c r="C61" s="2"/>
       <c r="D61" t="s" s="2">
@@ -9982,13 +9977,13 @@
         <v>50</v>
       </c>
       <c r="K61" t="s" s="2">
+        <v>488</v>
+      </c>
+      <c r="L61" t="s" s="2">
         <v>489</v>
       </c>
-      <c r="L61" t="s" s="2">
+      <c r="M61" t="s" s="2">
         <v>490</v>
-      </c>
-      <c r="M61" t="s" s="2">
-        <v>491</v>
       </c>
       <c r="N61" s="2"/>
       <c r="O61" s="2"/>
@@ -10039,7 +10034,7 @@
         <v>35</v>
       </c>
       <c r="AF61" t="s" s="2">
-        <v>488</v>
+        <v>487</v>
       </c>
       <c r="AG61" t="s" s="2">
         <v>36</v>
@@ -10057,22 +10052,22 @@
         <v>35</v>
       </c>
       <c r="AL61" t="s" s="2">
+        <v>491</v>
+      </c>
+      <c r="AM61" t="s" s="2">
         <v>492</v>
       </c>
-      <c r="AM61" t="s" s="2">
+      <c r="AN61" t="s" s="2">
         <v>493</v>
       </c>
-      <c r="AN61" t="s" s="2">
+      <c r="AO61" t="s" s="2">
+        <v>35</v>
+      </c>
+      <c r="AP61" t="s" s="2">
+        <v>35</v>
+      </c>
+      <c r="AQ61" t="s" s="2">
         <v>494</v>
-      </c>
-      <c r="AO61" t="s" s="2">
-        <v>35</v>
-      </c>
-      <c r="AP61" t="s" s="2">
-        <v>35</v>
-      </c>
-      <c r="AQ61" t="s" s="2">
-        <v>495</v>
       </c>
       <c r="AR61" t="s" s="2">
         <v>35</v>
@@ -10083,10 +10078,10 @@
     </row>
     <row r="62" hidden="true">
       <c r="A62" t="s" s="2">
-        <v>496</v>
+        <v>495</v>
       </c>
       <c r="B62" t="s" s="2">
-        <v>496</v>
+        <v>495</v>
       </c>
       <c r="C62" s="2"/>
       <c r="D62" t="s" s="2">
@@ -10210,10 +10205,10 @@
     </row>
     <row r="63" hidden="true">
       <c r="A63" t="s" s="2">
-        <v>497</v>
+        <v>496</v>
       </c>
       <c r="B63" t="s" s="2">
-        <v>497</v>
+        <v>496</v>
       </c>
       <c r="C63" s="2"/>
       <c r="D63" t="s" s="2">
@@ -10339,10 +10334,10 @@
     </row>
     <row r="64" hidden="true">
       <c r="A64" t="s" s="2">
-        <v>498</v>
+        <v>497</v>
       </c>
       <c r="B64" t="s" s="2">
-        <v>498</v>
+        <v>497</v>
       </c>
       <c r="C64" s="2"/>
       <c r="D64" t="s" s="2">
@@ -10365,16 +10360,16 @@
         <v>50</v>
       </c>
       <c r="K64" t="s" s="2">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="L64" t="s" s="2">
+        <v>498</v>
+      </c>
+      <c r="M64" t="s" s="2">
         <v>499</v>
       </c>
-      <c r="M64" t="s" s="2">
+      <c r="N64" t="s" s="2">
         <v>500</v>
-      </c>
-      <c r="N64" t="s" s="2">
-        <v>501</v>
       </c>
       <c r="O64" s="2"/>
       <c r="P64" t="s" s="2">
@@ -10424,16 +10419,16 @@
         <v>35</v>
       </c>
       <c r="AF64" t="s" s="2">
+        <v>501</v>
+      </c>
+      <c r="AG64" t="s" s="2">
+        <v>36</v>
+      </c>
+      <c r="AH64" t="s" s="2">
+        <v>49</v>
+      </c>
+      <c r="AI64" t="s" s="2">
         <v>502</v>
-      </c>
-      <c r="AG64" t="s" s="2">
-        <v>36</v>
-      </c>
-      <c r="AH64" t="s" s="2">
-        <v>49</v>
-      </c>
-      <c r="AI64" t="s" s="2">
-        <v>503</v>
       </c>
       <c r="AJ64" t="s" s="2">
         <v>83</v>
@@ -10445,33 +10440,33 @@
         <v>35</v>
       </c>
       <c r="AM64" t="s" s="2">
+        <v>503</v>
+      </c>
+      <c r="AN64" t="s" s="2">
+        <v>35</v>
+      </c>
+      <c r="AO64" t="s" s="2">
+        <v>35</v>
+      </c>
+      <c r="AP64" t="s" s="2">
         <v>504</v>
       </c>
-      <c r="AN64" t="s" s="2">
-        <v>35</v>
-      </c>
-      <c r="AO64" t="s" s="2">
-        <v>35</v>
-      </c>
-      <c r="AP64" t="s" s="2">
+      <c r="AQ64" t="s" s="2">
+        <v>35</v>
+      </c>
+      <c r="AR64" t="s" s="2">
         <v>505</v>
       </c>
-      <c r="AQ64" t="s" s="2">
-        <v>35</v>
-      </c>
-      <c r="AR64" t="s" s="2">
+      <c r="AS64" t="s" s="2">
         <v>506</v>
-      </c>
-      <c r="AS64" t="s" s="2">
-        <v>507</v>
       </c>
     </row>
     <row r="65" hidden="true">
       <c r="A65" t="s" s="2">
-        <v>508</v>
+        <v>507</v>
       </c>
       <c r="B65" t="s" s="2">
-        <v>508</v>
+        <v>507</v>
       </c>
       <c r="C65" s="2"/>
       <c r="D65" t="s" s="2">
@@ -10494,69 +10489,69 @@
         <v>50</v>
       </c>
       <c r="K65" t="s" s="2">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="L65" t="s" s="2">
+        <v>508</v>
+      </c>
+      <c r="M65" t="s" s="2">
         <v>509</v>
       </c>
-      <c r="M65" t="s" s="2">
+      <c r="N65" t="s" s="2">
         <v>510</v>
-      </c>
-      <c r="N65" t="s" s="2">
-        <v>511</v>
       </c>
       <c r="O65" s="2"/>
       <c r="P65" t="s" s="2">
         <v>35</v>
       </c>
       <c r="Q65" t="s" s="2">
+        <v>511</v>
+      </c>
+      <c r="R65" t="s" s="2">
+        <v>35</v>
+      </c>
+      <c r="S65" t="s" s="2">
+        <v>35</v>
+      </c>
+      <c r="T65" t="s" s="2">
+        <v>35</v>
+      </c>
+      <c r="U65" t="s" s="2">
+        <v>35</v>
+      </c>
+      <c r="V65" t="s" s="2">
+        <v>35</v>
+      </c>
+      <c r="W65" t="s" s="2">
+        <v>35</v>
+      </c>
+      <c r="X65" t="s" s="2">
+        <v>35</v>
+      </c>
+      <c r="Y65" t="s" s="2">
+        <v>35</v>
+      </c>
+      <c r="Z65" t="s" s="2">
+        <v>35</v>
+      </c>
+      <c r="AA65" t="s" s="2">
+        <v>35</v>
+      </c>
+      <c r="AB65" t="s" s="2">
+        <v>35</v>
+      </c>
+      <c r="AC65" t="s" s="2">
+        <v>35</v>
+      </c>
+      <c r="AD65" t="s" s="2">
+        <v>35</v>
+      </c>
+      <c r="AE65" t="s" s="2">
+        <v>35</v>
+      </c>
+      <c r="AF65" t="s" s="2">
         <v>512</v>
       </c>
-      <c r="R65" t="s" s="2">
-        <v>35</v>
-      </c>
-      <c r="S65" t="s" s="2">
-        <v>35</v>
-      </c>
-      <c r="T65" t="s" s="2">
-        <v>35</v>
-      </c>
-      <c r="U65" t="s" s="2">
-        <v>35</v>
-      </c>
-      <c r="V65" t="s" s="2">
-        <v>35</v>
-      </c>
-      <c r="W65" t="s" s="2">
-        <v>35</v>
-      </c>
-      <c r="X65" t="s" s="2">
-        <v>35</v>
-      </c>
-      <c r="Y65" t="s" s="2">
-        <v>35</v>
-      </c>
-      <c r="Z65" t="s" s="2">
-        <v>35</v>
-      </c>
-      <c r="AA65" t="s" s="2">
-        <v>35</v>
-      </c>
-      <c r="AB65" t="s" s="2">
-        <v>35</v>
-      </c>
-      <c r="AC65" t="s" s="2">
-        <v>35</v>
-      </c>
-      <c r="AD65" t="s" s="2">
-        <v>35</v>
-      </c>
-      <c r="AE65" t="s" s="2">
-        <v>35</v>
-      </c>
-      <c r="AF65" t="s" s="2">
-        <v>513</v>
-      </c>
       <c r="AG65" t="s" s="2">
         <v>36</v>
       </c>
@@ -10564,7 +10559,7 @@
         <v>49</v>
       </c>
       <c r="AI65" t="s" s="2">
-        <v>503</v>
+        <v>502</v>
       </c>
       <c r="AJ65" t="s" s="2">
         <v>83</v>
@@ -10576,33 +10571,33 @@
         <v>35</v>
       </c>
       <c r="AM65" t="s" s="2">
+        <v>513</v>
+      </c>
+      <c r="AN65" t="s" s="2">
+        <v>35</v>
+      </c>
+      <c r="AO65" t="s" s="2">
+        <v>35</v>
+      </c>
+      <c r="AP65" t="s" s="2">
         <v>514</v>
       </c>
-      <c r="AN65" t="s" s="2">
-        <v>35</v>
-      </c>
-      <c r="AO65" t="s" s="2">
-        <v>35</v>
-      </c>
-      <c r="AP65" t="s" s="2">
+      <c r="AQ65" t="s" s="2">
+        <v>35</v>
+      </c>
+      <c r="AR65" t="s" s="2">
         <v>515</v>
       </c>
-      <c r="AQ65" t="s" s="2">
-        <v>35</v>
-      </c>
-      <c r="AR65" t="s" s="2">
+      <c r="AS65" t="s" s="2">
         <v>516</v>
-      </c>
-      <c r="AS65" t="s" s="2">
-        <v>517</v>
       </c>
     </row>
     <row r="66" hidden="true">
       <c r="A66" t="s" s="2">
-        <v>518</v>
+        <v>517</v>
       </c>
       <c r="B66" t="s" s="2">
-        <v>518</v>
+        <v>517</v>
       </c>
       <c r="C66" s="2"/>
       <c r="D66" t="s" s="2">
@@ -10628,10 +10623,10 @@
         <v>210</v>
       </c>
       <c r="L66" t="s" s="2">
+        <v>518</v>
+      </c>
+      <c r="M66" t="s" s="2">
         <v>519</v>
-      </c>
-      <c r="M66" t="s" s="2">
-        <v>520</v>
       </c>
       <c r="N66" s="2"/>
       <c r="O66" s="2"/>
@@ -10661,75 +10656,75 @@
         <v>131</v>
       </c>
       <c r="Y66" t="s" s="2">
+        <v>520</v>
+      </c>
+      <c r="Z66" t="s" s="2">
         <v>521</v>
       </c>
-      <c r="Z66" t="s" s="2">
+      <c r="AA66" t="s" s="2">
+        <v>35</v>
+      </c>
+      <c r="AB66" t="s" s="2">
+        <v>35</v>
+      </c>
+      <c r="AC66" t="s" s="2">
+        <v>35</v>
+      </c>
+      <c r="AD66" t="s" s="2">
+        <v>35</v>
+      </c>
+      <c r="AE66" t="s" s="2">
+        <v>35</v>
+      </c>
+      <c r="AF66" t="s" s="2">
+        <v>517</v>
+      </c>
+      <c r="AG66" t="s" s="2">
+        <v>36</v>
+      </c>
+      <c r="AH66" t="s" s="2">
+        <v>49</v>
+      </c>
+      <c r="AI66" t="s" s="2">
+        <v>35</v>
+      </c>
+      <c r="AJ66" t="s" s="2">
         <v>522</v>
       </c>
-      <c r="AA66" t="s" s="2">
-        <v>35</v>
-      </c>
-      <c r="AB66" t="s" s="2">
-        <v>35</v>
-      </c>
-      <c r="AC66" t="s" s="2">
-        <v>35</v>
-      </c>
-      <c r="AD66" t="s" s="2">
-        <v>35</v>
-      </c>
-      <c r="AE66" t="s" s="2">
-        <v>35</v>
-      </c>
-      <c r="AF66" t="s" s="2">
-        <v>518</v>
-      </c>
-      <c r="AG66" t="s" s="2">
-        <v>36</v>
-      </c>
-      <c r="AH66" t="s" s="2">
-        <v>49</v>
-      </c>
-      <c r="AI66" t="s" s="2">
-        <v>35</v>
-      </c>
-      <c r="AJ66" t="s" s="2">
+      <c r="AK66" t="s" s="2">
+        <v>35</v>
+      </c>
+      <c r="AL66" t="s" s="2">
         <v>523</v>
       </c>
-      <c r="AK66" t="s" s="2">
-        <v>35</v>
-      </c>
-      <c r="AL66" t="s" s="2">
+      <c r="AM66" t="s" s="2">
         <v>524</v>
       </c>
-      <c r="AM66" t="s" s="2">
+      <c r="AN66" t="s" s="2">
         <v>525</v>
       </c>
-      <c r="AN66" t="s" s="2">
+      <c r="AO66" t="s" s="2">
+        <v>35</v>
+      </c>
+      <c r="AP66" t="s" s="2">
+        <v>35</v>
+      </c>
+      <c r="AQ66" t="s" s="2">
         <v>526</v>
       </c>
-      <c r="AO66" t="s" s="2">
-        <v>35</v>
-      </c>
-      <c r="AP66" t="s" s="2">
-        <v>35</v>
-      </c>
-      <c r="AQ66" t="s" s="2">
+      <c r="AR66" t="s" s="2">
+        <v>526</v>
+      </c>
+      <c r="AS66" t="s" s="2">
         <v>527</v>
-      </c>
-      <c r="AR66" t="s" s="2">
-        <v>527</v>
-      </c>
-      <c r="AS66" t="s" s="2">
-        <v>528</v>
       </c>
     </row>
     <row r="67" hidden="true">
       <c r="A67" t="s" s="2">
-        <v>529</v>
+        <v>528</v>
       </c>
       <c r="B67" t="s" s="2">
-        <v>529</v>
+        <v>528</v>
       </c>
       <c r="C67" s="2"/>
       <c r="D67" t="s" s="2">
@@ -10755,16 +10750,16 @@
         <v>210</v>
       </c>
       <c r="L67" t="s" s="2">
+        <v>529</v>
+      </c>
+      <c r="M67" t="s" s="2">
         <v>530</v>
       </c>
-      <c r="M67" t="s" s="2">
+      <c r="N67" t="s" s="2">
         <v>531</v>
       </c>
-      <c r="N67" t="s" s="2">
+      <c r="O67" t="s" s="2">
         <v>532</v>
-      </c>
-      <c r="O67" t="s" s="2">
-        <v>533</v>
       </c>
       <c r="P67" t="s" s="2">
         <v>35</v>
@@ -10792,75 +10787,75 @@
         <v>131</v>
       </c>
       <c r="Y67" t="s" s="2">
+        <v>533</v>
+      </c>
+      <c r="Z67" t="s" s="2">
         <v>534</v>
       </c>
-      <c r="Z67" t="s" s="2">
+      <c r="AA67" t="s" s="2">
+        <v>35</v>
+      </c>
+      <c r="AB67" t="s" s="2">
+        <v>35</v>
+      </c>
+      <c r="AC67" t="s" s="2">
+        <v>35</v>
+      </c>
+      <c r="AD67" t="s" s="2">
+        <v>35</v>
+      </c>
+      <c r="AE67" t="s" s="2">
+        <v>35</v>
+      </c>
+      <c r="AF67" t="s" s="2">
+        <v>528</v>
+      </c>
+      <c r="AG67" t="s" s="2">
+        <v>36</v>
+      </c>
+      <c r="AH67" t="s" s="2">
+        <v>49</v>
+      </c>
+      <c r="AI67" t="s" s="2">
+        <v>35</v>
+      </c>
+      <c r="AJ67" t="s" s="2">
+        <v>522</v>
+      </c>
+      <c r="AK67" t="s" s="2">
+        <v>35</v>
+      </c>
+      <c r="AL67" t="s" s="2">
+        <v>523</v>
+      </c>
+      <c r="AM67" t="s" s="2">
+        <v>524</v>
+      </c>
+      <c r="AN67" t="s" s="2">
+        <v>523</v>
+      </c>
+      <c r="AO67" t="s" s="2">
+        <v>35</v>
+      </c>
+      <c r="AP67" t="s" s="2">
+        <v>35</v>
+      </c>
+      <c r="AQ67" t="s" s="2">
         <v>535</v>
       </c>
-      <c r="AA67" t="s" s="2">
-        <v>35</v>
-      </c>
-      <c r="AB67" t="s" s="2">
-        <v>35</v>
-      </c>
-      <c r="AC67" t="s" s="2">
-        <v>35</v>
-      </c>
-      <c r="AD67" t="s" s="2">
-        <v>35</v>
-      </c>
-      <c r="AE67" t="s" s="2">
-        <v>35</v>
-      </c>
-      <c r="AF67" t="s" s="2">
-        <v>529</v>
-      </c>
-      <c r="AG67" t="s" s="2">
-        <v>36</v>
-      </c>
-      <c r="AH67" t="s" s="2">
-        <v>49</v>
-      </c>
-      <c r="AI67" t="s" s="2">
-        <v>35</v>
-      </c>
-      <c r="AJ67" t="s" s="2">
-        <v>523</v>
-      </c>
-      <c r="AK67" t="s" s="2">
-        <v>35</v>
-      </c>
-      <c r="AL67" t="s" s="2">
-        <v>524</v>
-      </c>
-      <c r="AM67" t="s" s="2">
-        <v>525</v>
-      </c>
-      <c r="AN67" t="s" s="2">
-        <v>524</v>
-      </c>
-      <c r="AO67" t="s" s="2">
-        <v>35</v>
-      </c>
-      <c r="AP67" t="s" s="2">
-        <v>35</v>
-      </c>
-      <c r="AQ67" t="s" s="2">
+      <c r="AR67" t="s" s="2">
+        <v>535</v>
+      </c>
+      <c r="AS67" t="s" s="2">
         <v>536</v>
-      </c>
-      <c r="AR67" t="s" s="2">
-        <v>536</v>
-      </c>
-      <c r="AS67" t="s" s="2">
-        <v>537</v>
       </c>
     </row>
     <row r="68" hidden="true">
       <c r="A68" t="s" s="2">
-        <v>538</v>
+        <v>537</v>
       </c>
       <c r="B68" t="s" s="2">
-        <v>538</v>
+        <v>537</v>
       </c>
       <c r="C68" s="2"/>
       <c r="D68" t="s" s="2">
@@ -10883,13 +10878,13 @@
         <v>35</v>
       </c>
       <c r="K68" t="s" s="2">
+        <v>538</v>
+      </c>
+      <c r="L68" t="s" s="2">
         <v>539</v>
       </c>
-      <c r="L68" t="s" s="2">
+      <c r="M68" t="s" s="2">
         <v>540</v>
-      </c>
-      <c r="M68" t="s" s="2">
-        <v>541</v>
       </c>
       <c r="N68" s="2"/>
       <c r="O68" s="2"/>
@@ -10940,7 +10935,7 @@
         <v>35</v>
       </c>
       <c r="AF68" t="s" s="2">
-        <v>538</v>
+        <v>537</v>
       </c>
       <c r="AG68" t="s" s="2">
         <v>36</v>
@@ -10958,14 +10953,14 @@
         <v>35</v>
       </c>
       <c r="AL68" t="s" s="2">
+        <v>245</v>
+      </c>
+      <c r="AM68" t="s" s="2">
         <v>246</v>
       </c>
-      <c r="AM68" t="s" s="2">
+      <c r="AN68" t="s" s="2">
         <v>247</v>
       </c>
-      <c r="AN68" t="s" s="2">
-        <v>248</v>
-      </c>
       <c r="AO68" t="s" s="2">
         <v>35</v>
       </c>
@@ -10973,7 +10968,7 @@
         <v>35</v>
       </c>
       <c r="AQ68" t="s" s="2">
-        <v>542</v>
+        <v>541</v>
       </c>
       <c r="AR68" t="s" s="2">
         <v>35</v>
@@ -10984,10 +10979,10 @@
     </row>
     <row r="69" hidden="true">
       <c r="A69" t="s" s="2">
-        <v>543</v>
+        <v>542</v>
       </c>
       <c r="B69" t="s" s="2">
-        <v>543</v>
+        <v>542</v>
       </c>
       <c r="C69" s="2"/>
       <c r="D69" t="s" s="2">
@@ -11111,10 +11106,10 @@
     </row>
     <row r="70" hidden="true">
       <c r="A70" t="s" s="2">
-        <v>544</v>
+        <v>543</v>
       </c>
       <c r="B70" t="s" s="2">
-        <v>544</v>
+        <v>543</v>
       </c>
       <c r="C70" s="2"/>
       <c r="D70" t="s" s="2">
@@ -11240,10 +11235,10 @@
     </row>
     <row r="71" hidden="true">
       <c r="A71" t="s" s="2">
-        <v>545</v>
+        <v>544</v>
       </c>
       <c r="B71" t="s" s="2">
-        <v>545</v>
+        <v>544</v>
       </c>
       <c r="C71" s="2"/>
       <c r="D71" t="s" s="2">
@@ -11269,13 +11264,13 @@
         <v>62</v>
       </c>
       <c r="L71" t="s" s="2">
+        <v>545</v>
+      </c>
+      <c r="M71" t="s" s="2">
         <v>546</v>
       </c>
-      <c r="M71" t="s" s="2">
+      <c r="N71" t="s" s="2">
         <v>547</v>
-      </c>
-      <c r="N71" t="s" s="2">
-        <v>548</v>
       </c>
       <c r="O71" s="2"/>
       <c r="P71" t="s" s="2">
@@ -11325,16 +11320,16 @@
         <v>35</v>
       </c>
       <c r="AF71" t="s" s="2">
+        <v>548</v>
+      </c>
+      <c r="AG71" t="s" s="2">
+        <v>36</v>
+      </c>
+      <c r="AH71" t="s" s="2">
+        <v>49</v>
+      </c>
+      <c r="AI71" t="s" s="2">
         <v>549</v>
-      </c>
-      <c r="AG71" t="s" s="2">
-        <v>36</v>
-      </c>
-      <c r="AH71" t="s" s="2">
-        <v>49</v>
-      </c>
-      <c r="AI71" t="s" s="2">
-        <v>550</v>
       </c>
       <c r="AJ71" t="s" s="2">
         <v>83</v>
@@ -11361,7 +11356,7 @@
         <v>35</v>
       </c>
       <c r="AR71" t="s" s="2">
-        <v>551</v>
+        <v>550</v>
       </c>
       <c r="AS71" t="s" s="2">
         <v>35</v>
@@ -11369,10 +11364,10 @@
     </row>
     <row r="72" hidden="true">
       <c r="A72" t="s" s="2">
-        <v>552</v>
+        <v>551</v>
       </c>
       <c r="B72" t="s" s="2">
-        <v>552</v>
+        <v>551</v>
       </c>
       <c r="C72" s="2"/>
       <c r="D72" t="s" s="2">
@@ -11398,13 +11393,13 @@
         <v>92</v>
       </c>
       <c r="L72" t="s" s="2">
+        <v>552</v>
+      </c>
+      <c r="M72" t="s" s="2">
         <v>553</v>
       </c>
-      <c r="M72" t="s" s="2">
+      <c r="N72" t="s" s="2">
         <v>554</v>
-      </c>
-      <c r="N72" t="s" s="2">
-        <v>555</v>
       </c>
       <c r="O72" s="2"/>
       <c r="P72" t="s" s="2">
@@ -11433,28 +11428,28 @@
         <v>109</v>
       </c>
       <c r="Y72" t="s" s="2">
+        <v>555</v>
+      </c>
+      <c r="Z72" t="s" s="2">
         <v>556</v>
       </c>
-      <c r="Z72" t="s" s="2">
+      <c r="AA72" t="s" s="2">
+        <v>35</v>
+      </c>
+      <c r="AB72" t="s" s="2">
+        <v>35</v>
+      </c>
+      <c r="AC72" t="s" s="2">
+        <v>35</v>
+      </c>
+      <c r="AD72" t="s" s="2">
+        <v>35</v>
+      </c>
+      <c r="AE72" t="s" s="2">
+        <v>35</v>
+      </c>
+      <c r="AF72" t="s" s="2">
         <v>557</v>
-      </c>
-      <c r="AA72" t="s" s="2">
-        <v>35</v>
-      </c>
-      <c r="AB72" t="s" s="2">
-        <v>35</v>
-      </c>
-      <c r="AC72" t="s" s="2">
-        <v>35</v>
-      </c>
-      <c r="AD72" t="s" s="2">
-        <v>35</v>
-      </c>
-      <c r="AE72" t="s" s="2">
-        <v>35</v>
-      </c>
-      <c r="AF72" t="s" s="2">
-        <v>558</v>
       </c>
       <c r="AG72" t="s" s="2">
         <v>36</v>
@@ -11498,10 +11493,10 @@
     </row>
     <row r="73" hidden="true">
       <c r="A73" t="s" s="2">
-        <v>559</v>
+        <v>558</v>
       </c>
       <c r="B73" t="s" s="2">
-        <v>559</v>
+        <v>558</v>
       </c>
       <c r="C73" s="2"/>
       <c r="D73" t="s" s="2">
@@ -11527,13 +11522,13 @@
         <v>175</v>
       </c>
       <c r="L73" t="s" s="2">
+        <v>559</v>
+      </c>
+      <c r="M73" t="s" s="2">
         <v>560</v>
       </c>
-      <c r="M73" t="s" s="2">
+      <c r="N73" t="s" s="2">
         <v>561</v>
-      </c>
-      <c r="N73" t="s" s="2">
-        <v>562</v>
       </c>
       <c r="O73" s="2"/>
       <c r="P73" t="s" s="2">
@@ -11583,7 +11578,7 @@
         <v>35</v>
       </c>
       <c r="AF73" t="s" s="2">
-        <v>563</v>
+        <v>562</v>
       </c>
       <c r="AG73" t="s" s="2">
         <v>36</v>
@@ -11604,22 +11599,22 @@
         <v>35</v>
       </c>
       <c r="AM73" t="s" s="2">
+        <v>563</v>
+      </c>
+      <c r="AN73" t="s" s="2">
+        <v>35</v>
+      </c>
+      <c r="AO73" t="s" s="2">
+        <v>35</v>
+      </c>
+      <c r="AP73" t="s" s="2">
+        <v>35</v>
+      </c>
+      <c r="AQ73" t="s" s="2">
+        <v>35</v>
+      </c>
+      <c r="AR73" t="s" s="2">
         <v>564</v>
-      </c>
-      <c r="AN73" t="s" s="2">
-        <v>35</v>
-      </c>
-      <c r="AO73" t="s" s="2">
-        <v>35</v>
-      </c>
-      <c r="AP73" t="s" s="2">
-        <v>35</v>
-      </c>
-      <c r="AQ73" t="s" s="2">
-        <v>35</v>
-      </c>
-      <c r="AR73" t="s" s="2">
-        <v>565</v>
       </c>
       <c r="AS73" t="s" s="2">
         <v>35</v>
@@ -11627,10 +11622,10 @@
     </row>
     <row r="74" hidden="true">
       <c r="A74" t="s" s="2">
-        <v>566</v>
+        <v>565</v>
       </c>
       <c r="B74" t="s" s="2">
-        <v>566</v>
+        <v>565</v>
       </c>
       <c r="C74" s="2"/>
       <c r="D74" t="s" s="2">
@@ -11656,13 +11651,13 @@
         <v>62</v>
       </c>
       <c r="L74" t="s" s="2">
+        <v>566</v>
+      </c>
+      <c r="M74" t="s" s="2">
         <v>567</v>
       </c>
-      <c r="M74" t="s" s="2">
+      <c r="N74" t="s" s="2">
         <v>568</v>
-      </c>
-      <c r="N74" t="s" s="2">
-        <v>569</v>
       </c>
       <c r="O74" s="2"/>
       <c r="P74" t="s" s="2">
@@ -11712,7 +11707,7 @@
         <v>35</v>
       </c>
       <c r="AF74" t="s" s="2">
-        <v>570</v>
+        <v>569</v>
       </c>
       <c r="AG74" t="s" s="2">
         <v>36</v>
@@ -11756,10 +11751,10 @@
     </row>
     <row r="75" hidden="true">
       <c r="A75" t="s" s="2">
-        <v>571</v>
+        <v>570</v>
       </c>
       <c r="B75" t="s" s="2">
-        <v>571</v>
+        <v>570</v>
       </c>
       <c r="C75" s="2"/>
       <c r="D75" t="s" s="2">
@@ -11782,16 +11777,16 @@
         <v>35</v>
       </c>
       <c r="K75" t="s" s="2">
+        <v>571</v>
+      </c>
+      <c r="L75" t="s" s="2">
         <v>572</v>
       </c>
-      <c r="L75" t="s" s="2">
+      <c r="M75" t="s" s="2">
         <v>573</v>
       </c>
-      <c r="M75" t="s" s="2">
+      <c r="N75" t="s" s="2">
         <v>574</v>
-      </c>
-      <c r="N75" t="s" s="2">
-        <v>575</v>
       </c>
       <c r="O75" s="2"/>
       <c r="P75" t="s" s="2">
@@ -11841,7 +11836,7 @@
         <v>35</v>
       </c>
       <c r="AF75" t="s" s="2">
-        <v>571</v>
+        <v>570</v>
       </c>
       <c r="AG75" t="s" s="2">
         <v>36</v>
@@ -11859,25 +11854,25 @@
         <v>35</v>
       </c>
       <c r="AL75" t="s" s="2">
+        <v>575</v>
+      </c>
+      <c r="AM75" t="s" s="2">
         <v>576</v>
       </c>
-      <c r="AM75" t="s" s="2">
+      <c r="AN75" t="s" s="2">
         <v>577</v>
       </c>
-      <c r="AN75" t="s" s="2">
+      <c r="AO75" t="s" s="2">
+        <v>35</v>
+      </c>
+      <c r="AP75" t="s" s="2">
+        <v>35</v>
+      </c>
+      <c r="AQ75" t="s" s="2">
         <v>578</v>
       </c>
-      <c r="AO75" t="s" s="2">
-        <v>35</v>
-      </c>
-      <c r="AP75" t="s" s="2">
-        <v>35</v>
-      </c>
-      <c r="AQ75" t="s" s="2">
+      <c r="AR75" t="s" s="2">
         <v>579</v>
-      </c>
-      <c r="AR75" t="s" s="2">
-        <v>580</v>
       </c>
       <c r="AS75" t="s" s="2">
         <v>35</v>

</xml_diff>